<commit_message>
body full need to work on quartiles
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/Updated_full_Filtered_Data_with_real_length.xlsx
+++ b/fifty_one/measurements/Updated_full_Filtered_Data_with_real_length.xlsx
@@ -616,7 +616,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S2" t="n">
-        <v>18.41245121697855</v>
+        <v>89.46024071800146</v>
       </c>
       <c r="T2" t="n">
         <v>89.51942722609853</v>
@@ -699,7 +699,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S3" t="n">
-        <v>28.54325445641133</v>
+        <v>144.8515207401151</v>
       </c>
       <c r="T3" t="n">
         <v>144.8764102773935</v>
@@ -782,7 +782,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S4" t="n">
-        <v>27.40005145522436</v>
+        <v>128.7456511458256</v>
       </c>
       <c r="T4" t="n">
         <v>128.7456516191202</v>
@@ -865,7 +865,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S5" t="n">
-        <v>25.64095843222629</v>
+        <v>150.6240150220556</v>
       </c>
       <c r="T5" t="n">
         <v>150.6240311294727</v>
@@ -948,7 +948,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S6" t="n">
-        <v>21.16636442904771</v>
+        <v>119.5420748666193</v>
       </c>
       <c r="T6" t="n">
         <v>119.5420482817262</v>
@@ -1031,7 +1031,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S7" t="n">
-        <v>23.37339306123902</v>
+        <v>172.420065508728</v>
       </c>
       <c r="T7" t="n">
         <v>172.4200714868299</v>
@@ -1114,7 +1114,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S8" t="n">
-        <v>14.55250640515562</v>
+        <v>113.6408664857839</v>
       </c>
       <c r="T8" t="n">
         <v>113.6408665105316</v>
@@ -1197,7 +1197,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S9" t="n">
-        <v>25.82935467005808</v>
+        <v>138.2698349929292</v>
       </c>
       <c r="T9" t="n">
         <v>138.3169991723383</v>
@@ -1280,7 +1280,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S10" t="n">
-        <v>29.0267023603768</v>
+        <v>142.7588110864231</v>
       </c>
       <c r="T10" t="n">
         <v>142.7588103148251</v>
@@ -1363,10 +1363,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S11" t="n">
-        <v>19.62293856317094</v>
+        <v>151.0657175583403</v>
       </c>
       <c r="T11" t="n">
-        <v>151.0819118574266</v>
+        <v>151.0819118574265</v>
       </c>
       <c r="U11" t="n">
         <v>138.8704192860928</v>
@@ -1446,7 +1446,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S12" t="n">
-        <v>33.50150189142796</v>
+        <v>156.6829076672418</v>
       </c>
       <c r="T12" t="n">
         <v>156.6829120200248</v>
@@ -1529,7 +1529,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S13" t="n">
-        <v>21.65042716454379</v>
+        <v>144.6045711003246</v>
       </c>
       <c r="T13" t="n">
         <v>144.6045605979157</v>
@@ -1612,7 +1612,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S14" t="n">
-        <v>18.50868419588127</v>
+        <v>126.5207712080109</v>
       </c>
       <c r="T14" t="n">
         <v>126.5207646060668</v>
@@ -1695,7 +1695,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S15" t="n">
-        <v>13.85415775568651</v>
+        <v>108.345930129826</v>
       </c>
       <c r="T15" t="n">
         <v>108.3459220829687</v>
@@ -1778,7 +1778,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S16" t="n">
-        <v>23.67546465386005</v>
+        <v>140.2892118969358</v>
       </c>
       <c r="T16" t="n">
         <v>140.2892015392351</v>
@@ -1861,7 +1861,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S17" t="n">
-        <v>17.04506653184843</v>
+        <v>137.5702402908112</v>
       </c>
       <c r="T17" t="n">
         <v>137.5702402908112</v>
@@ -1944,7 +1944,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S18" t="n">
-        <v>30.72391368233249</v>
+        <v>160.977943256303</v>
       </c>
       <c r="T18" t="n">
         <v>161.048122716919</v>
@@ -2027,7 +2027,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S19" t="n">
-        <v>26.63288931417365</v>
+        <v>125.1874920747535</v>
       </c>
       <c r="T19" t="n">
         <v>125.1874738028053</v>
@@ -2110,7 +2110,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S20" t="n">
-        <v>23.58383705493082</v>
+        <v>111.2409289861498</v>
       </c>
       <c r="T20" t="n">
         <v>111.2409241572751</v>
@@ -2193,7 +2193,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S21" t="n">
-        <v>20.77099353743314</v>
+        <v>105.1295408502361</v>
       </c>
       <c r="T21" t="n">
         <v>105.1295426559788</v>
@@ -2276,7 +2276,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S22" t="n">
-        <v>28.79820509097973</v>
+        <v>159.9830878636595</v>
       </c>
       <c r="T22" t="n">
         <v>160.0528242681144</v>
@@ -2359,7 +2359,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S23" t="n">
-        <v>27.34258413210752</v>
+        <v>127.9012207178111</v>
       </c>
       <c r="T23" t="n">
         <v>127.926016180156</v>
@@ -2442,7 +2442,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S24" t="n">
-        <v>15.54011149455156</v>
+        <v>124.6644626264112</v>
       </c>
       <c r="T24" t="n">
         <v>124.7183536330472</v>
@@ -2525,7 +2525,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S25" t="n">
-        <v>24.7507926115887</v>
+        <v>120.8475082815099</v>
       </c>
       <c r="T25" t="n">
         <v>120.8475065438441</v>
@@ -2608,7 +2608,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S26" t="n">
-        <v>29.08211450567878</v>
+        <v>149.3150667423094</v>
       </c>
       <c r="T26" t="n">
         <v>149.6863841228801</v>
@@ -2691,7 +2691,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S27" t="n">
-        <v>24.88575251975895</v>
+        <v>138.1017777427979</v>
       </c>
       <c r="T27" t="n">
         <v>138.101764458228</v>
@@ -2774,7 +2774,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S28" t="n">
-        <v>29.72220221716891</v>
+        <v>147.1120482341852</v>
       </c>
       <c r="T28" t="n">
         <v>147.1120501204356</v>
@@ -2857,7 +2857,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S29" t="n">
-        <v>28.32980502772372</v>
+        <v>152.2574242428964</v>
       </c>
       <c r="T29" t="n">
         <v>152.5047429966486</v>
@@ -2940,7 +2940,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S30" t="n">
-        <v>29.49407373149284</v>
+        <v>140.2091023664197</v>
       </c>
       <c r="T30" t="n">
         <v>140.2097111148776</v>
@@ -3023,7 +3023,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S31" t="n">
-        <v>31.97243473320157</v>
+        <v>149.6444809088116</v>
       </c>
       <c r="T31" t="n">
         <v>149.6444801727167</v>
@@ -3106,7 +3106,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S32" t="n">
-        <v>22.57516028438255</v>
+        <v>138.4699501156378</v>
       </c>
       <c r="T32" t="n">
         <v>138.4699417984678</v>
@@ -3189,7 +3189,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S33" t="n">
-        <v>31.41718273426304</v>
+        <v>147.2719024438159</v>
       </c>
       <c r="T33" t="n">
         <v>147.2719071129475</v>
@@ -3272,7 +3272,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S34" t="n">
-        <v>27.81031088260993</v>
+        <v>148.7515533854336</v>
       </c>
       <c r="T34" t="n">
         <v>148.7515712806191</v>
@@ -3355,7 +3355,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S35" t="n">
-        <v>30.07315070071706</v>
+        <v>152.7024814839053</v>
       </c>
       <c r="T35" t="n">
         <v>152.7024702983286</v>
@@ -3438,7 +3438,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S36" t="n">
-        <v>22.30715965838933</v>
+        <v>121.5263359659202</v>
       </c>
       <c r="T36" t="n">
         <v>121.5263478147821</v>
@@ -3521,7 +3521,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S37" t="n">
-        <v>31.78085963655306</v>
+        <v>156.2107008267397</v>
       </c>
       <c r="T37" t="n">
         <v>156.210702417082</v>
@@ -3604,7 +3604,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S38" t="n">
-        <v>28.15945775465657</v>
+        <v>164.4066251729149</v>
       </c>
       <c r="T38" t="n">
         <v>164.4066206824926</v>
@@ -3687,7 +3687,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S39" t="n">
-        <v>21.42358890528796</v>
+        <v>122.3649338174221</v>
       </c>
       <c r="T39" t="n">
         <v>122.3649644815153</v>
@@ -3770,7 +3770,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S40" t="n">
-        <v>24.35358445878079</v>
+        <v>142.6385953299745</v>
       </c>
       <c r="T40" t="n">
         <v>142.638588527619</v>
@@ -3853,7 +3853,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S41" t="n">
-        <v>26.68495078820414</v>
+        <v>176.7490859304091</v>
       </c>
       <c r="T41" t="n">
         <v>176.7490786984841</v>
@@ -3936,7 +3936,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S42" t="n">
-        <v>29.81668889749374</v>
+        <v>151.0383143758084</v>
       </c>
       <c r="T42" t="n">
         <v>151.1346091349536</v>
@@ -4019,7 +4019,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S43" t="n">
-        <v>24.95703727047621</v>
+        <v>162.1486827172921</v>
       </c>
       <c r="T43" t="n">
         <v>162.1486797571503</v>
@@ -4102,7 +4102,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S44" t="n">
-        <v>24.52622115712974</v>
+        <v>125.4214795218226</v>
       </c>
       <c r="T44" t="n">
         <v>125.4214734450268</v>
@@ -4185,7 +4185,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S45" t="n">
-        <v>25.58098626072759</v>
+        <v>149.2712769645643</v>
       </c>
       <c r="T45" t="n">
         <v>149.2713046606348</v>
@@ -4268,7 +4268,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S46" t="n">
-        <v>33.35258221588032</v>
+        <v>162.0554097753725</v>
       </c>
       <c r="T46" t="n">
         <v>162.0554129223326</v>
@@ -4351,7 +4351,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S47" t="n">
-        <v>29.09038541709339</v>
+        <v>141.8480799296507</v>
       </c>
       <c r="T47" t="n">
         <v>141.8480810531717</v>
@@ -4434,7 +4434,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S48" t="n">
-        <v>29.68482205370279</v>
+        <v>142.3129925323429</v>
       </c>
       <c r="T48" t="n">
         <v>142.3130100217776</v>
@@ -4517,7 +4517,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S49" t="n">
-        <v>17.0743545412518</v>
+        <v>126.6843998844925</v>
       </c>
       <c r="T49" t="n">
         <v>126.6843952890806</v>
@@ -4600,7 +4600,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S50" t="n">
-        <v>19.69166071528478</v>
+        <v>98.72581894307027</v>
       </c>
       <c r="T50" t="n">
         <v>98.725831638765</v>
@@ -4683,7 +4683,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S51" t="n">
-        <v>22.30964823207185</v>
+        <v>170.2539310229063</v>
       </c>
       <c r="T51" t="n">
         <v>170.2539528140297</v>
@@ -4766,7 +4766,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S52" t="n">
-        <v>22.14396683935574</v>
+        <v>131.4215357211992</v>
       </c>
       <c r="T52" t="n">
         <v>131.4215437639736</v>
@@ -4849,7 +4849,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S53" t="n">
-        <v>21.24316191353668</v>
+        <v>173.683960951193</v>
       </c>
       <c r="T53" t="n">
         <v>173.6839335289665</v>
@@ -4932,7 +4932,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S54" t="n">
-        <v>18.86518635827786</v>
+        <v>154.3387098881642</v>
       </c>
       <c r="T54" t="n">
         <v>154.3387472073479</v>
@@ -5015,7 +5015,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S55" t="n">
-        <v>12.79157818923693</v>
+        <v>104.5489069764239</v>
       </c>
       <c r="T55" t="n">
         <v>104.5489072588774</v>
@@ -5098,7 +5098,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S56" t="n">
-        <v>33.42408002721034</v>
+        <v>157.4718495938019</v>
       </c>
       <c r="T56" t="n">
         <v>157.4718411178839</v>
@@ -5181,7 +5181,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S57" t="n">
-        <v>26.93413215562246</v>
+        <v>155.1543536278412</v>
       </c>
       <c r="T57" t="n">
         <v>155.1570088198594</v>
@@ -5264,7 +5264,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S58" t="n">
-        <v>21.71955032183897</v>
+        <v>131.5555759651063</v>
       </c>
       <c r="T58" t="n">
         <v>131.555613020363</v>
@@ -5347,10 +5347,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S59" t="n">
-        <v>25.29289635124608</v>
+        <v>135.3455984320063</v>
       </c>
       <c r="T59" t="n">
-        <v>135.3489985181046</v>
+        <v>135.3489985181045</v>
       </c>
       <c r="U59" t="n">
         <v>144.4524383673576</v>
@@ -5430,7 +5430,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S60" t="n">
-        <v>28.46469876301014</v>
+        <v>137.3777892051259</v>
       </c>
       <c r="T60" t="n">
         <v>137.3777835275524</v>
@@ -5513,7 +5513,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S61" t="n">
-        <v>32.54892278448008</v>
+        <v>152.3293516906985</v>
       </c>
       <c r="T61" t="n">
         <v>152.3293653376577</v>
@@ -5596,7 +5596,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S62" t="n">
-        <v>20.55245855042843</v>
+        <v>143.361146868522</v>
       </c>
       <c r="T62" t="n">
         <v>143.3611511582353</v>
@@ -5679,7 +5679,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S63" t="n">
-        <v>15.24799842392614</v>
+        <v>115.6114747377499</v>
       </c>
       <c r="T63" t="n">
         <v>115.6114879590968</v>
@@ -5762,7 +5762,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S64" t="n">
-        <v>31.40304305711093</v>
+        <v>158.9306635251178</v>
       </c>
       <c r="T64" t="n">
         <v>158.9306472803991</v>
@@ -5845,10 +5845,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S65" t="n">
-        <v>31.63787932898325</v>
+        <v>158.5730751243332</v>
       </c>
       <c r="T65" t="n">
-        <v>159.0812954077794</v>
+        <v>159.0812954077793</v>
       </c>
       <c r="U65" t="n">
         <v>179.5172317571584</v>
@@ -5928,7 +5928,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S66" t="n">
-        <v>28.09037083324632</v>
+        <v>131.1734859929433</v>
       </c>
       <c r="T66" t="n">
         <v>131.1734960698861</v>
@@ -6011,7 +6011,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S67" t="n">
-        <v>27.81563368487555</v>
+        <v>130.993419510247</v>
       </c>
       <c r="T67" t="n">
         <v>130.9934248061256</v>
@@ -6094,7 +6094,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S68" t="n">
-        <v>27.64144849100096</v>
+        <v>140.8871156880767</v>
       </c>
       <c r="T68" t="n">
         <v>140.8871140911096</v>
@@ -6177,7 +6177,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S69" t="n">
-        <v>30.55177264313123</v>
+        <v>145.7185652068018</v>
       </c>
       <c r="T69" t="n">
         <v>145.7193915989705</v>
@@ -6260,7 +6260,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S70" t="n">
-        <v>32.45782889157297</v>
+        <v>154.814545864654</v>
       </c>
       <c r="T70" t="n">
         <v>154.8145436392874</v>
@@ -6343,7 +6343,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S71" t="n">
-        <v>32.85224695485368</v>
+        <v>164.5993746850113</v>
       </c>
       <c r="T71" t="n">
         <v>164.5993620866842</v>
@@ -6426,7 +6426,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S72" t="n">
-        <v>17.93282750246336</v>
+        <v>147.5192352325103</v>
       </c>
       <c r="T72" t="n">
         <v>147.5192165237457</v>
@@ -6509,7 +6509,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S73" t="n">
-        <v>24.69765115362</v>
+        <v>139.5163781825055</v>
       </c>
       <c r="T73" t="n">
         <v>139.5296578303904</v>
@@ -6592,7 +6592,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S74" t="n">
-        <v>24.51716532131686</v>
+        <v>126.2824911787496</v>
       </c>
       <c r="T74" t="n">
         <v>126.2824925669569</v>
@@ -6675,10 +6675,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S75" t="n">
-        <v>26.9031966830677</v>
+        <v>137.1857168428197</v>
       </c>
       <c r="T75" t="n">
-        <v>137.1914186316164</v>
+        <v>137.1914186316166</v>
       </c>
       <c r="U75" t="n">
         <v>150.6326631752464</v>
@@ -6758,7 +6758,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S76" t="n">
-        <v>18.85341156069364</v>
+        <v>102.3670734810906</v>
       </c>
       <c r="T76" t="n">
         <v>102.3687556197054</v>
@@ -6841,7 +6841,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S77" t="n">
-        <v>18.01992677740402</v>
+        <v>95.4494967802917</v>
       </c>
       <c r="T77" t="n">
         <v>95.44948698425914</v>
@@ -6924,7 +6924,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S78" t="n">
-        <v>23.64489673940236</v>
+        <v>112.711544803459</v>
       </c>
       <c r="T78" t="n">
         <v>112.7125218760619</v>
@@ -7007,7 +7007,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S79" t="n">
-        <v>14.54990272161832</v>
+        <v>77.14872675419424</v>
       </c>
       <c r="T79" t="n">
         <v>77.14872089159915</v>
@@ -7090,7 +7090,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S80" t="n">
-        <v>22.39078954748982</v>
+        <v>159.4404491733029</v>
       </c>
       <c r="T80" t="n">
         <v>159.4404373403439</v>
@@ -7173,7 +7173,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S81" t="n">
-        <v>22.17700859030642</v>
+        <v>106.5699815665904</v>
       </c>
       <c r="T81" t="n">
         <v>106.6482381960493</v>
@@ -7256,7 +7256,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S82" t="n">
-        <v>26.77760899515397</v>
+        <v>125.534312116556</v>
       </c>
       <c r="T82" t="n">
         <v>125.5342987354669</v>
@@ -7339,7 +7339,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S83" t="n">
-        <v>12.64479212977603</v>
+        <v>78.51469192480864</v>
       </c>
       <c r="T83" t="n">
         <v>78.51466666678633</v>
@@ -7422,7 +7422,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S84" t="n">
-        <v>21.00840427801247</v>
+        <v>112.6233162331283</v>
       </c>
       <c r="T84" t="n">
         <v>112.6288123011965</v>
@@ -7505,7 +7505,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S85" t="n">
-        <v>19.48001787525633</v>
+        <v>142.4081273057455</v>
       </c>
       <c r="T85" t="n">
         <v>142.4852494498875</v>
@@ -7588,7 +7588,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S86" t="n">
-        <v>19.38574304382326</v>
+        <v>139.6295518806741</v>
       </c>
       <c r="T86" t="n">
         <v>139.6295391577229</v>
@@ -7671,7 +7671,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S87" t="n">
-        <v>28.75769357876141</v>
+        <v>137.0950371659708</v>
       </c>
       <c r="T87" t="n">
         <v>137.0950394225367</v>
@@ -7754,7 +7754,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S88" t="n">
-        <v>23.66373735289095</v>
+        <v>147.3238543538565</v>
       </c>
       <c r="T88" t="n">
         <v>147.3332230805846</v>
@@ -7837,7 +7837,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S89" t="n">
-        <v>17.2897579680757</v>
+        <v>131.7702941780663</v>
       </c>
       <c r="T89" t="n">
         <v>131.7702936017997</v>
@@ -7920,7 +7920,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S90" t="n">
-        <v>32.74900250288449</v>
+        <v>158.9828288591914</v>
       </c>
       <c r="T90" t="n">
         <v>158.982777363679</v>
@@ -8003,7 +8003,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S91" t="n">
-        <v>29.30524123578117</v>
+        <v>137.4543016877627</v>
       </c>
       <c r="T91" t="n">
         <v>137.454320347847</v>
@@ -8086,10 +8086,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S92" t="n">
-        <v>19.7367174866672</v>
+        <v>162.0819696043318</v>
       </c>
       <c r="T92" t="n">
-        <v>162.0844743691948</v>
+        <v>162.0844743691949</v>
       </c>
       <c r="U92" t="n">
         <v>150.2256353241279</v>
@@ -8169,7 +8169,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S93" t="n">
-        <v>23.13465542868036</v>
+        <v>147.6398930750444</v>
       </c>
       <c r="T93" t="n">
         <v>147.6398826298108</v>
@@ -8252,7 +8252,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S94" t="n">
-        <v>18.21236485740626</v>
+        <v>109.8294039681047</v>
       </c>
       <c r="T94" t="n">
         <v>109.8294017744384</v>
@@ -8335,7 +8335,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S95" t="n">
-        <v>34.33785215023558</v>
+        <v>163.1651446563927</v>
       </c>
       <c r="T95" t="n">
         <v>163.1651451777951</v>
@@ -8418,7 +8418,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S96" t="n">
-        <v>23.66608327798498</v>
+        <v>189.914075188585</v>
       </c>
       <c r="T96" t="n">
         <v>189.9140575512969</v>
@@ -8501,7 +8501,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S97" t="n">
-        <v>17.5921514010218</v>
+        <v>145.4419045162077</v>
       </c>
       <c r="T97" t="n">
         <v>145.4418954359053</v>
@@ -8584,7 +8584,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S98" t="n">
-        <v>30.76303902295018</v>
+        <v>145.4617369487765</v>
       </c>
       <c r="T98" t="n">
         <v>145.4617186198604</v>
@@ -8667,7 +8667,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S99" t="n">
-        <v>18.16352714305956</v>
+        <v>139.3324832457644</v>
       </c>
       <c r="T99" t="n">
         <v>139.4680625119909</v>
@@ -8750,7 +8750,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S100" t="n">
-        <v>24.45746403642546</v>
+        <v>125.5296090040163</v>
       </c>
       <c r="T100" t="n">
         <v>125.5296221627943</v>
@@ -8833,7 +8833,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S101" t="n">
-        <v>27.0157685953061</v>
+        <v>178.16852955447</v>
       </c>
       <c r="T101" t="n">
         <v>178.1685316380975</v>
@@ -8916,10 +8916,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S102" t="n">
-        <v>22.77330385012174</v>
+        <v>117.2452579198594</v>
       </c>
       <c r="T102" t="n">
-        <v>117.4176474462011</v>
+        <v>117.417647446201</v>
       </c>
       <c r="U102" t="n">
         <v>127.3152845818141</v>
@@ -8999,10 +8999,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S103" t="n">
-        <v>22.77330385012174</v>
+        <v>117.2452579198594</v>
       </c>
       <c r="T103" t="n">
-        <v>117.4176474462011</v>
+        <v>117.417647446201</v>
       </c>
       <c r="U103" t="n">
         <v>127.3152845818141</v>
@@ -9082,10 +9082,10 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S104" t="n">
-        <v>22.77330385012174</v>
+        <v>117.2452579198594</v>
       </c>
       <c r="T104" t="n">
-        <v>117.4176474462011</v>
+        <v>117.417647446201</v>
       </c>
       <c r="U104" t="n">
         <v>127.3152845818141</v>
@@ -9165,7 +9165,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S105" t="n">
-        <v>18.00774133563472</v>
+        <v>97.72762860224847</v>
       </c>
       <c r="T105" t="n">
         <v>97.72765587960151</v>
@@ -9248,7 +9248,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S106" t="n">
-        <v>18.85329540180989</v>
+        <v>96.10923874915792</v>
       </c>
       <c r="T106" t="n">
         <v>96.10923874915792</v>
@@ -9331,7 +9331,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S107" t="n">
-        <v>31.57885671919704</v>
+        <v>170.6383557080179</v>
       </c>
       <c r="T107" t="n">
         <v>170.7023610360049</v>
@@ -9414,7 +9414,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S108" t="n">
-        <v>15.27596861124021</v>
+        <v>82.38096485731846</v>
       </c>
       <c r="T108" t="n">
         <v>82.38097332039634</v>
@@ -9497,7 +9497,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S109" t="n">
-        <v>22.46010008329068</v>
+        <v>135.5852100746213</v>
       </c>
       <c r="T109" t="n">
         <v>135.5851928333629</v>
@@ -9580,7 +9580,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S110" t="n">
-        <v>17.64800172886985</v>
+        <v>117.5144461663911</v>
       </c>
       <c r="T110" t="n">
         <v>117.514428742831</v>
@@ -9663,7 +9663,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S111" t="n">
-        <v>28.39115567834585</v>
+        <v>136.3662613294278</v>
       </c>
       <c r="T111" t="n">
         <v>136.3662532363129</v>
@@ -9821,7 +9821,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S113" t="n">
-        <v>19.34497746417141</v>
+        <v>108.216371425595</v>
       </c>
       <c r="T113" t="n">
         <v>108.2163726288793</v>
@@ -9979,7 +9979,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S115" t="n">
-        <v>13.67427653360674</v>
+        <v>111.7734305806518</v>
       </c>
       <c r="T115" t="n">
         <v>111.7734371893911</v>
@@ -10062,7 +10062,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S116" t="n">
-        <v>26.47656152431712</v>
+        <v>128.015088802559</v>
       </c>
       <c r="T116" t="n">
         <v>128.0150974087073</v>
@@ -10445,7 +10445,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S121" t="n">
-        <v>22.96040234120882</v>
+        <v>122.1170856974565</v>
       </c>
       <c r="T121" t="n">
         <v>122.1170781881949</v>
@@ -10528,7 +10528,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S122" t="n">
-        <v>15.13015886499415</v>
+        <v>111.84505655063</v>
       </c>
       <c r="T122" t="n">
         <v>111.8450418414499</v>
@@ -10911,7 +10911,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S127" t="n">
-        <v>25.65074194580773</v>
+        <v>122.129358640651</v>
       </c>
       <c r="T127" t="n">
         <v>122.1293534970989</v>
@@ -10994,7 +10994,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S128" t="n">
-        <v>17.00708372979112</v>
+        <v>131.4562610781874</v>
       </c>
       <c r="T128" t="n">
         <v>131.4562840030627</v>
@@ -11077,7 +11077,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S129" t="n">
-        <v>21.2288290415306</v>
+        <v>160.8436791632326</v>
       </c>
       <c r="T129" t="n">
         <v>160.8436677165517</v>
@@ -11160,7 +11160,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S130" t="n">
-        <v>17.68452957799136</v>
+        <v>144.9115492470041</v>
       </c>
       <c r="T130" t="n">
         <v>144.9115225839679</v>
@@ -11243,7 +11243,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S131" t="n">
-        <v>13.74661507186937</v>
+        <v>104.4993706470194</v>
       </c>
       <c r="T131" t="n">
         <v>104.4993706470194</v>
@@ -11326,7 +11326,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S132" t="n">
-        <v>22.35840974149103</v>
+        <v>162.0556869657647</v>
       </c>
       <c r="T132" t="n">
         <v>162.0556845677155</v>
@@ -11409,7 +11409,7 @@
         <v>1.230960202536279</v>
       </c>
       <c r="S133" t="n">
-        <v>19.58285581624185</v>
+        <v>141.7639396357654</v>
       </c>
       <c r="T133" t="n">
         <v>141.7639407002064</v>

</xml_diff>

<commit_message>
with pixels in excel
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/Updated_full_Filtered_Data_with_real_length.xlsx
+++ b/fifty_one/measurements/Updated_full_Filtered_Data_with_real_length.xlsx
@@ -1366,7 +1366,7 @@
         <v>151.0657175583403</v>
       </c>
       <c r="T11" t="n">
-        <v>151.0819118574265</v>
+        <v>151.0819118574266</v>
       </c>
       <c r="U11" t="n">
         <v>138.8704192860928</v>
@@ -5184,7 +5184,7 @@
         <v>155.1543536278412</v>
       </c>
       <c r="T57" t="n">
-        <v>155.1570088198594</v>
+        <v>155.1570088198592</v>
       </c>
       <c r="U57" t="n">
         <v>172.1115825104016</v>
@@ -6512,7 +6512,7 @@
         <v>139.5163781825055</v>
       </c>
       <c r="T73" t="n">
-        <v>139.5296578303904</v>
+        <v>139.5296578303906</v>
       </c>
       <c r="U73" t="n">
         <v>146.6056405622281</v>
@@ -8089,7 +8089,7 @@
         <v>162.0819696043318</v>
       </c>
       <c r="T92" t="n">
-        <v>162.0844743691949</v>
+        <v>162.0844743691948</v>
       </c>
       <c r="U92" t="n">
         <v>150.2256353241279</v>

</xml_diff>

<commit_message>
finished for now with body visuals
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/Updated_full_Filtered_Data_with_real_length.xlsx
+++ b/fifty_one/measurements/Updated_full_Filtered_Data_with_real_length.xlsx
@@ -665,28 +665,28 @@
         <v>87.32366386173278</v>
       </c>
       <c r="V2" t="n">
-        <v>98.63224100852604</v>
+        <v>74.76470624280951</v>
       </c>
       <c r="W2" t="n">
-        <v>87.38143681982831</v>
+        <v>87.38143681982832</v>
       </c>
       <c r="X2" t="n">
         <v>465.0141732779099</v>
       </c>
       <c r="Y2" t="n">
-        <v>525.234375</v>
+        <v>398.135471261432</v>
       </c>
       <c r="Z2" t="n">
-        <v>465.3218246424834</v>
+        <v>465.3218246424835</v>
       </c>
       <c r="AA2" t="n">
         <v>87.65076982969236</v>
       </c>
       <c r="AB2" t="n">
-        <v>87.70875919968067</v>
+        <v>87.70875919968069</v>
       </c>
       <c r="AC2" t="n">
-        <v>99.00170780870752</v>
+        <v>75.04476757467819</v>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
@@ -772,19 +772,19 @@
         <v>141.3920352264977</v>
       </c>
       <c r="V3" t="n">
-        <v>161.9517043720242</v>
+        <v>132.2260097199337</v>
       </c>
       <c r="W3" t="n">
-        <v>141.416330327534</v>
+        <v>141.4163303275339</v>
       </c>
       <c r="X3" t="n">
         <v>752.9379490196103</v>
       </c>
       <c r="Y3" t="n">
-        <v>862.421875</v>
+        <v>704.1272190904584</v>
       </c>
       <c r="Z3" t="n">
-        <v>753.0673247904319</v>
+        <v>753.0673247904316</v>
       </c>
       <c r="AA3" t="n">
         <v>141.921676064951</v>
@@ -793,7 +793,7 @@
         <v>141.9460621730773</v>
       </c>
       <c r="AC3" t="n">
-        <v>162.5583597352852</v>
+        <v>132.7213155166232</v>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         <v>125.6708217425546</v>
       </c>
       <c r="V4" t="n">
-        <v>168.0401143108221</v>
+        <v>122.1976242665746</v>
       </c>
       <c r="W4" t="n">
         <v>125.6708222045455</v>
@@ -888,7 +888,7 @@
         <v>669.2196673092043</v>
       </c>
       <c r="Y4" t="n">
-        <v>894.84375</v>
+        <v>650.7242677634285</v>
       </c>
       <c r="Z4" t="n">
         <v>669.219669769389</v>
@@ -900,7 +900,7 @@
         <v>126.1415729051412</v>
       </c>
       <c r="AC4" t="n">
-        <v>168.6695762666869</v>
+        <v>122.6553647048522</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
@@ -986,7 +986,7 @@
         <v>147.0266651612517</v>
       </c>
       <c r="V5" t="n">
-        <v>137.5980646168326</v>
+        <v>131.3789820895892</v>
       </c>
       <c r="W5" t="n">
         <v>147.0266808839757</v>
@@ -995,7 +995,7 @@
         <v>782.9433641037203</v>
       </c>
       <c r="Y5" t="n">
-        <v>732.734375</v>
+        <v>699.6166450278322</v>
       </c>
       <c r="Z5" t="n">
         <v>782.9434478300459</v>
@@ -1007,7 +1007,7 @@
         <v>147.5774285580837</v>
       </c>
       <c r="AC5" t="n">
-        <v>138.1134936096784</v>
+        <v>131.8711150029997</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
@@ -1093,7 +1093,7 @@
         <v>116.6870542623771</v>
       </c>
       <c r="V6" t="n">
-        <v>104.7206509473239</v>
+        <v>97.83623074704535</v>
       </c>
       <c r="W6" t="n">
         <v>116.6870283124104</v>
@@ -1102,7 +1102,7 @@
         <v>621.3794940621174</v>
       </c>
       <c r="Y6" t="n">
-        <v>557.65625</v>
+        <v>520.995477577541</v>
       </c>
       <c r="Z6" t="n">
         <v>621.3793558738898</v>
@@ -1114,7 +1114,7 @@
         <v>117.1241265931799</v>
       </c>
       <c r="AC6" t="n">
-        <v>105.1129243401092</v>
+        <v>98.20271577005931</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
@@ -1200,7 +1200,7 @@
         <v>168.3021610791668</v>
       </c>
       <c r="V7" t="n">
-        <v>132.7273366657943</v>
+        <v>138.3698287686405</v>
       </c>
       <c r="W7" t="n">
         <v>168.3021669144937</v>
@@ -1209,7 +1209,7 @@
         <v>896.2391960446696</v>
       </c>
       <c r="Y7" t="n">
-        <v>706.796875</v>
+        <v>736.8441575394352</v>
       </c>
       <c r="Z7" t="n">
         <v>896.2392271188326</v>
@@ -1221,7 +1221,7 @@
         <v>168.9326104939733</v>
       </c>
       <c r="AC7" t="n">
-        <v>133.224520384557</v>
+        <v>138.8881487150806</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
@@ -1307,7 +1307,7 @@
         <v>110.9267843045699</v>
       </c>
       <c r="V8" t="n">
-        <v>71.84323727781526</v>
+        <v>77.26073897646847</v>
       </c>
       <c r="W8" t="n">
         <v>110.9267843287265</v>
@@ -1316,7 +1316,7 @@
         <v>590.7050233192431</v>
       </c>
       <c r="Y8" t="n">
-        <v>382.578125</v>
+        <v>411.4272932806598</v>
       </c>
       <c r="Z8" t="n">
         <v>590.7050234478816</v>
@@ -1328,7 +1328,7 @@
         <v>111.3423052947037</v>
       </c>
       <c r="AC8" t="n">
-        <v>72.11235507054005</v>
+        <v>77.5501502046573</v>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
@@ -1414,7 +1414,7 @@
         <v>134.9675397275138</v>
       </c>
       <c r="V9" t="n">
-        <v>142.4687925678709</v>
+        <v>124.2640596500611</v>
       </c>
       <c r="W9" t="n">
         <v>135.0135774859187</v>
@@ -1423,7 +1423,7 @@
         <v>718.7263581280739</v>
       </c>
       <c r="Y9" t="n">
-        <v>758.671875</v>
+        <v>661.7284068362659</v>
       </c>
       <c r="Z9" t="n">
         <v>718.9715174493565</v>
@@ -1435,7 +1435,7 @@
         <v>135.5193252408589</v>
       </c>
       <c r="AC9" t="n">
-        <v>143.0024668347998</v>
+        <v>124.7295407546879</v>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
@@ -1521,7 +1521,7 @@
         <v>139.3493057089765</v>
       </c>
       <c r="V10" t="n">
-        <v>165.604750335303</v>
+        <v>128.653324736496</v>
       </c>
       <c r="W10" t="n">
         <v>139.3493049558066</v>
@@ -1530,7 +1530,7 @@
         <v>742.0600479351514</v>
       </c>
       <c r="Y10" t="n">
-        <v>881.875</v>
+        <v>685.1020307224317</v>
       </c>
       <c r="Z10" t="n">
         <v>742.0600439243865</v>
@@ -1542,7 +1542,7 @@
         <v>139.8712939249621</v>
       </c>
       <c r="AC10" t="n">
-        <v>166.2250896541262</v>
+        <v>129.1352476020526</v>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
@@ -1628,7 +1628,7 @@
         <v>147.4578185260966</v>
       </c>
       <c r="V11" t="n">
-        <v>102.2852869718048</v>
+        <v>128.0286754852751</v>
       </c>
       <c r="W11" t="n">
         <v>147.4736260571129</v>
@@ -1637,7 +1637,7 @@
         <v>785.2393331073433</v>
       </c>
       <c r="Y11" t="n">
-        <v>544.6875</v>
+        <v>681.7756614165692</v>
       </c>
       <c r="Z11" t="n">
         <v>785.3235110453966</v>
@@ -1649,7 +1649,7 @@
         <v>148.0260479444527</v>
       </c>
       <c r="AC11" t="n">
-        <v>102.6684377275486</v>
+        <v>128.508258475374</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
@@ -1735,7 +1735,7 @@
         <v>152.9408534137777</v>
       </c>
       <c r="V12" t="n">
-        <v>209.4413018946479</v>
+        <v>151.1919147648076</v>
       </c>
       <c r="W12" t="n">
         <v>152.9408576626033</v>
@@ -1744,7 +1744,7 @@
         <v>814.4374773742417</v>
       </c>
       <c r="Y12" t="n">
-        <v>1115.3125</v>
+        <v>805.124065361979</v>
       </c>
       <c r="Z12" t="n">
         <v>814.4375000000001</v>
@@ -1756,7 +1756,7 @@
         <v>153.5137592688107</v>
       </c>
       <c r="AC12" t="n">
-        <v>210.2258486802184</v>
+        <v>151.7582650006968</v>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
@@ -1842,7 +1842,7 @@
         <v>141.1509834792325</v>
       </c>
       <c r="V13" t="n">
-        <v>105.9383329350835</v>
+        <v>125.1488976079331</v>
       </c>
       <c r="W13" t="n">
         <v>141.1509732276523</v>
@@ -1851,7 +1851,7 @@
         <v>751.6543052280576</v>
       </c>
       <c r="Y13" t="n">
-        <v>564.140625</v>
+        <v>666.4403276750007</v>
       </c>
       <c r="Z13" t="n">
         <v>751.6542506365545</v>
@@ -1863,7 +1863,7 @@
         <v>141.6797110712588</v>
       </c>
       <c r="AC13" t="n">
-        <v>106.3351676463896</v>
+        <v>125.6176932296553</v>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>123.4990785607441</v>
       </c>
       <c r="V14" t="n">
-        <v>75.49628324109401</v>
+        <v>102.8037492387761</v>
       </c>
       <c r="W14" t="n">
         <v>123.4990721164741</v>
@@ -1958,7 +1958,7 @@
         <v>657.65474532127</v>
       </c>
       <c r="Y14" t="n">
-        <v>402.03125</v>
+        <v>547.4484045680127</v>
       </c>
       <c r="Z14" t="n">
         <v>657.6547110043766</v>
@@ -1970,7 +1970,7 @@
         <v>123.9616876520606</v>
       </c>
       <c r="AC14" t="n">
-        <v>75.77908498938106</v>
+        <v>103.1888421038427</v>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
@@ -2056,7 +2056,7 @@
         <v>105.7583067909172</v>
       </c>
       <c r="V15" t="n">
-        <v>64.53714535125778</v>
+        <v>83.73573264114532</v>
       </c>
       <c r="W15" t="n">
         <v>105.7582989362429</v>
@@ -2065,7 +2065,7 @@
         <v>563.1819534910899</v>
       </c>
       <c r="Y15" t="n">
-        <v>343.671875</v>
+        <v>445.907795962349</v>
       </c>
       <c r="Z15" t="n">
         <v>563.1819116635403</v>
@@ -2077,7 +2077,7 @@
         <v>106.154459257666</v>
       </c>
       <c r="AC15" t="n">
-        <v>64.77889523285802</v>
+        <v>84.04939856704782</v>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
@@ -2163,7 +2163,7 @@
         <v>136.938687899711</v>
       </c>
       <c r="V16" t="n">
-        <v>125.4212447392368</v>
+        <v>117.9593776088418</v>
       </c>
       <c r="W16" t="n">
         <v>136.9386777893831</v>
@@ -2172,7 +2172,7 @@
         <v>729.2230757091629</v>
       </c>
       <c r="Y16" t="n">
-        <v>667.890625</v>
+        <v>628.1548440982227</v>
       </c>
       <c r="Z16" t="n">
         <v>729.223021869853</v>
@@ -2184,7 +2184,7 @@
         <v>137.4516367831826</v>
       </c>
       <c r="AC16" t="n">
-        <v>125.891060546875</v>
+        <v>118.4012419865636</v>
       </c>
       <c r="AD16" t="inlineStr">
         <is>
@@ -2270,7 +2270,7 @@
         <v>134.2846534294568</v>
       </c>
       <c r="V17" t="n">
-        <v>85.23773914317064</v>
+        <v>109.584754508139</v>
       </c>
       <c r="W17" t="n">
         <v>134.2846534294568</v>
@@ -2279,7 +2279,7 @@
         <v>715.0898661018505</v>
       </c>
       <c r="Y17" t="n">
-        <v>453.90625</v>
+        <v>583.5584739338465</v>
       </c>
       <c r="Z17" t="n">
         <v>715.0898661018505</v>
@@ -2291,7 +2291,7 @@
         <v>134.7876707056411</v>
       </c>
       <c r="AC17" t="n">
-        <v>85.55703143962378</v>
+        <v>109.9952483606846</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
@@ -2377,28 +2377,28 @@
         <v>157.1333107673816</v>
       </c>
       <c r="V18" t="n">
-        <v>178.9992522006584</v>
+        <v>149.0554807383192</v>
       </c>
       <c r="W18" t="n">
-        <v>157.2018141335658</v>
+        <v>157.201814133566</v>
       </c>
       <c r="X18" t="n">
         <v>836.7630647817501</v>
       </c>
       <c r="Y18" t="n">
-        <v>953.203125</v>
+        <v>793.7471709595254</v>
       </c>
       <c r="Z18" t="n">
-        <v>837.127857494105</v>
+        <v>837.1278574941061</v>
       </c>
       <c r="AA18" t="n">
         <v>157.7219168959409</v>
       </c>
       <c r="AB18" t="n">
-        <v>157.7906768690848</v>
+        <v>157.790676869085</v>
       </c>
       <c r="AC18" t="n">
-        <v>179.6697660232099</v>
+        <v>149.6138280997377</v>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
@@ -2484,7 +2484,7 @@
         <v>122.1976421021342</v>
       </c>
       <c r="V19" t="n">
-        <v>161.9517043720242</v>
+        <v>117.2700155373638</v>
       </c>
       <c r="W19" t="n">
         <v>122.1976242665745</v>
@@ -2493,7 +2493,7 @@
         <v>650.7243627409828</v>
       </c>
       <c r="Y19" t="n">
-        <v>862.421875</v>
+        <v>624.4838674169756</v>
       </c>
       <c r="Z19" t="n">
         <v>650.7242677634282</v>
@@ -2505,7 +2505,7 @@
         <v>122.6553647048521</v>
       </c>
       <c r="AC19" t="n">
-        <v>162.5583597352852</v>
+        <v>117.709297631685</v>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
@@ -2591,7 +2591,7 @@
         <v>108.5841644566328</v>
       </c>
       <c r="V20" t="n">
-        <v>140.0334285923518</v>
+        <v>101.016643147634</v>
       </c>
       <c r="W20" t="n">
         <v>108.584159743086</v>
@@ -2600,7 +2600,7 @@
         <v>578.2301524340984</v>
       </c>
       <c r="Y20" t="n">
-        <v>745.703125</v>
+        <v>537.9317440801041</v>
       </c>
       <c r="Z20" t="n">
         <v>578.2301273336162</v>
@@ -2612,7 +2612,7 @@
         <v>108.9909054647735</v>
       </c>
       <c r="AC20" t="n">
-        <v>140.5579802222391</v>
+        <v>101.3950416867649</v>
       </c>
       <c r="AD20" t="inlineStr">
         <is>
@@ -2698,7 +2698,7 @@
         <v>102.6187344619679</v>
       </c>
       <c r="V21" t="n">
-        <v>114.4621068494006</v>
+        <v>91.83728812922089</v>
       </c>
       <c r="W21" t="n">
         <v>102.6187362245841</v>
@@ -2707,7 +2707,7 @@
         <v>546.463167695475</v>
       </c>
       <c r="Y21" t="n">
-        <v>609.53125</v>
+        <v>489.0500321094459</v>
       </c>
       <c r="Z21" t="n">
         <v>546.4631770817224</v>
@@ -2719,7 +2719,7 @@
         <v>103.0031360488595</v>
       </c>
       <c r="AC21" t="n">
-        <v>114.8908707903519</v>
+        <v>92.18130169553048</v>
       </c>
       <c r="AD21" t="inlineStr">
         <is>
@@ -2805,28 +2805,28 @@
         <v>156.1622154830298</v>
       </c>
       <c r="V22" t="n">
-        <v>158.2986584087455</v>
+        <v>142.6150474863387</v>
       </c>
       <c r="W22" t="n">
-        <v>156.2302863745531</v>
+        <v>156.2302863745529</v>
       </c>
       <c r="X22" t="n">
         <v>831.5918082075649</v>
       </c>
       <c r="Y22" t="n">
-        <v>842.96875</v>
+        <v>759.4507086745327</v>
       </c>
       <c r="Z22" t="n">
-        <v>831.9542979147774</v>
+        <v>831.9542979147767</v>
       </c>
       <c r="AA22" t="n">
         <v>156.7471839829221</v>
       </c>
       <c r="AB22" t="n">
-        <v>156.815509861397</v>
+        <v>156.8155098613969</v>
       </c>
       <c r="AC22" t="n">
-        <v>158.8916298164442</v>
+        <v>143.1492696099945</v>
       </c>
       <c r="AD22" t="inlineStr">
         <is>
@@ -2912,28 +2912,28 @@
         <v>124.8465588268868</v>
       </c>
       <c r="V23" t="n">
-        <v>164.3870683475434</v>
+        <v>114.1672449182469</v>
       </c>
       <c r="W23" t="n">
-        <v>124.870762099779</v>
+        <v>124.8707620997791</v>
       </c>
       <c r="X23" t="n">
         <v>664.8303194355309</v>
       </c>
       <c r="Y23" t="n">
-        <v>875.390625</v>
+        <v>607.9610573273278</v>
       </c>
       <c r="Z23" t="n">
-        <v>664.9592062050143</v>
+        <v>664.9592062050144</v>
       </c>
       <c r="AA23" t="n">
         <v>125.3142219168845</v>
       </c>
       <c r="AB23" t="n">
-        <v>125.3385158528874</v>
+        <v>125.3385158528875</v>
       </c>
       <c r="AC23" t="n">
-        <v>165.0028463478459</v>
+        <v>114.5949043350276</v>
       </c>
       <c r="AD23" t="inlineStr">
         <is>
@@ -3019,7 +3019,7 @@
         <v>121.687104153988</v>
       </c>
       <c r="V24" t="n">
-        <v>93.76151305748772</v>
+        <v>109.5847545081391</v>
       </c>
       <c r="W24" t="n">
         <v>121.7397080829612</v>
@@ -3028,7 +3028,7 @@
         <v>648.0056565920962</v>
       </c>
       <c r="Y24" t="n">
-        <v>499.296875</v>
+        <v>583.5584739338469</v>
       </c>
       <c r="Z24" t="n">
         <v>648.2857819494262</v>
@@ -3040,7 +3040,7 @@
         <v>122.1957332116668</v>
       </c>
       <c r="AC24" t="n">
-        <v>94.11273458358617</v>
+        <v>109.9952483606847</v>
       </c>
       <c r="AD24" t="inlineStr">
         <is>
@@ -3126,7 +3126,7 @@
         <v>117.9613100412668</v>
       </c>
       <c r="V25" t="n">
-        <v>140.0334285923518</v>
+        <v>107.007531963467</v>
       </c>
       <c r="W25" t="n">
         <v>117.9613083451017</v>
@@ -3135,7 +3135,7 @@
         <v>628.165134647506</v>
       </c>
       <c r="Y25" t="n">
-        <v>745.703125</v>
+        <v>569.8343016079873</v>
       </c>
       <c r="Z25" t="n">
         <v>628.1651256151224</v>
@@ -3147,7 +3147,7 @@
         <v>118.4031799551741</v>
       </c>
       <c r="AC25" t="n">
-        <v>140.5579802222391</v>
+        <v>107.4083717905418</v>
       </c>
       <c r="AD25" t="inlineStr">
         <is>
@@ -3233,7 +3233,7 @@
         <v>145.7489784629422</v>
       </c>
       <c r="V26" t="n">
-        <v>168.0401143108221</v>
+        <v>138.3117967366042</v>
       </c>
       <c r="W26" t="n">
         <v>146.1114276791162</v>
@@ -3242,7 +3242,7 @@
         <v>776.139453257019</v>
       </c>
       <c r="Y26" t="n">
-        <v>894.84375</v>
+        <v>736.5351265596571</v>
       </c>
       <c r="Z26" t="n">
         <v>778.0695603455308</v>
@@ -3254,7 +3254,7 @@
         <v>146.6587469035662</v>
       </c>
       <c r="AC26" t="n">
-        <v>168.6695762666869</v>
+        <v>138.8298993006857</v>
       </c>
       <c r="AD26" t="inlineStr">
         <is>
@@ -3340,7 +3340,7 @@
         <v>134.8034961847935</v>
       </c>
       <c r="V27" t="n">
-        <v>131.5096546780347</v>
+        <v>117.1313970136564</v>
       </c>
       <c r="W27" t="n">
         <v>134.8034832174986</v>
@@ -3349,7 +3349,7 @@
         <v>717.8527968386568</v>
       </c>
       <c r="Y27" t="n">
-        <v>700.3125</v>
+        <v>623.7456989142789</v>
       </c>
       <c r="Z27" t="n">
         <v>717.8527277854857</v>
@@ -3361,7 +3361,7 @@
         <v>135.308443979704</v>
       </c>
       <c r="AC27" t="n">
-        <v>132.0022770782767</v>
+        <v>117.5701598564441</v>
       </c>
       <c r="AD27" t="inlineStr">
         <is>
@@ -3447,7 +3447,7 @@
         <v>143.5985745948034</v>
       </c>
       <c r="V28" t="n">
-        <v>177.7815702128988</v>
+        <v>138.5388472684103</v>
       </c>
       <c r="W28" t="n">
         <v>143.5985764360046</v>
@@ -3456,7 +3456,7 @@
         <v>764.6881669420113</v>
       </c>
       <c r="Y28" t="n">
-        <v>946.71875</v>
+        <v>737.744211367497</v>
       </c>
       <c r="Z28" t="n">
         <v>764.6881767467377</v>
@@ -3468,7 +3468,7 @@
         <v>144.1364827636307</v>
       </c>
       <c r="AC28" t="n">
-        <v>178.4475227169296</v>
+        <v>139.0578003417432</v>
       </c>
       <c r="AD28" t="inlineStr">
         <is>
@@ -3554,7 +3554,7 @@
         <v>148.6210637075173</v>
       </c>
       <c r="V29" t="n">
-        <v>160.7340223842646</v>
+        <v>144.0202353673912</v>
       </c>
       <c r="W29" t="n">
         <v>148.862475753204</v>
@@ -3563,7 +3563,7 @@
         <v>791.4338223492784</v>
       </c>
       <c r="Y29" t="n">
-        <v>855.9375</v>
+        <v>766.9335861891824</v>
       </c>
       <c r="Z29" t="n">
         <v>792.719384794552</v>
@@ -3575,7 +3575,7 @@
         <v>149.420100136684</v>
       </c>
       <c r="AC29" t="n">
-        <v>161.3361164290048</v>
+        <v>144.5597211884421</v>
       </c>
       <c r="AD29" t="inlineStr">
         <is>
@@ -3661,7 +3661,7 @@
         <v>136.8604916232561</v>
       </c>
       <c r="V30" t="n">
-        <v>165.604750335303</v>
+        <v>122.1440286444172</v>
       </c>
       <c r="W30" t="n">
         <v>136.8610858329887</v>
@@ -3670,7 +3670,7 @@
         <v>728.8066665110024</v>
       </c>
       <c r="Y30" t="n">
-        <v>881.875</v>
+        <v>650.4388614620131</v>
       </c>
       <c r="Z30" t="n">
         <v>728.8098307844116</v>
@@ -3682,7 +3682,7 @@
         <v>137.3737541748517</v>
       </c>
       <c r="AC30" t="n">
-        <v>166.2250896541262</v>
+        <v>122.601568318697</v>
       </c>
       <c r="AD30" t="inlineStr">
         <is>
@@ -3768,7 +3768,7 @@
         <v>146.0705252385384</v>
       </c>
       <c r="V31" t="n">
-        <v>193.6114360537733</v>
+        <v>139.8265451330602</v>
       </c>
       <c r="W31" t="n">
         <v>146.0705245200236</v>
@@ -3777,7 +3777,7 @@
         <v>777.8517475127978</v>
       </c>
       <c r="Y31" t="n">
-        <v>1031.015625</v>
+        <v>744.6014334706605</v>
       </c>
       <c r="Z31" t="n">
         <v>777.8517436865782</v>
@@ -3789,7 +3789,7 @@
         <v>146.6176905252103</v>
       </c>
       <c r="AC31" t="n">
-        <v>194.3366856985741</v>
+        <v>140.350321797592</v>
       </c>
       <c r="AD31" t="inlineStr">
         <is>
@@ -3875,7 +3875,7 @@
         <v>135.1628755053834</v>
       </c>
       <c r="V32" t="n">
-        <v>109.5913788983623</v>
+        <v>116.601605581278</v>
       </c>
       <c r="W32" t="n">
         <v>135.1628673868522</v>
@@ -3884,7 +3884,7 @@
         <v>719.7665561825377</v>
       </c>
       <c r="Y32" t="n">
-        <v>583.59375</v>
+        <v>620.9244645083653</v>
       </c>
       <c r="Z32" t="n">
         <v>719.7665129499028</v>
@@ -3896,7 +3896,7 @@
         <v>135.6691743672691</v>
       </c>
       <c r="AC32" t="n">
-        <v>110.0018975652306</v>
+        <v>117.038383876789</v>
       </c>
       <c r="AD32" t="inlineStr">
         <is>
@@ -3982,7 +3982,7 @@
         <v>143.7546110100494</v>
       </c>
       <c r="V33" t="n">
-        <v>182.6522981639371</v>
+        <v>129.7936318496911</v>
       </c>
       <c r="W33" t="n">
         <v>143.7546155676683</v>
@@ -3991,7 +3991,7 @@
         <v>765.5190888413919</v>
       </c>
       <c r="Y33" t="n">
-        <v>972.65625</v>
+        <v>691.1743706366724</v>
       </c>
       <c r="Z33" t="n">
         <v>765.5191131115297</v>
@@ -4003,7 +4003,7 @@
         <v>144.2931064027342</v>
       </c>
       <c r="AC33" t="n">
-        <v>183.336495942051</v>
+        <v>130.2798261949994</v>
       </c>
       <c r="AD33" t="inlineStr">
         <is>
@@ -4089,7 +4089,7 @@
         <v>145.198923482512</v>
       </c>
       <c r="V34" t="n">
-        <v>146.1218385311497</v>
+        <v>128.1993362163265</v>
       </c>
       <c r="W34" t="n">
         <v>145.1989409503072</v>
@@ -4098,7 +4098,7 @@
         <v>773.2103118230642</v>
       </c>
       <c r="Y34" t="n">
-        <v>778.125</v>
+        <v>682.6844604207715</v>
       </c>
       <c r="Z34" t="n">
         <v>773.2104048422069</v>
@@ -4110,7 +4110,7 @@
         <v>145.74284208805</v>
       </c>
       <c r="AC34" t="n">
-        <v>146.6691967536408</v>
+        <v>128.6795584849571</v>
       </c>
       <c r="AD34" t="inlineStr">
         <is>
@@ -4196,7 +4196,7 @@
         <v>149.0554916567512</v>
       </c>
       <c r="V35" t="n">
-        <v>172.9108422618605</v>
+        <v>140.6183461625234</v>
       </c>
       <c r="W35" t="n">
         <v>149.0554807383193</v>
@@ -4205,7 +4205,7 @@
         <v>793.7472291021342</v>
       </c>
       <c r="Y35" t="n">
-        <v>920.78125</v>
+        <v>748.8179159776178</v>
       </c>
       <c r="Z35" t="n">
         <v>793.7471709595259</v>
@@ -4217,7 +4217,7 @@
         <v>149.6138280997378</v>
       </c>
       <c r="AC35" t="n">
-        <v>173.5585494918082</v>
+        <v>141.1450888368481</v>
       </c>
       <c r="AD35" t="inlineStr">
         <is>
@@ -4303,7 +4303,7 @@
         <v>118.6239252998188</v>
       </c>
       <c r="V36" t="n">
-        <v>125.4212447392368</v>
+        <v>110.8262623198196</v>
       </c>
       <c r="W36" t="n">
         <v>118.6239368656947</v>
@@ -4312,7 +4312,7 @@
         <v>631.6936797523559</v>
       </c>
       <c r="Y36" t="n">
-        <v>667.890625</v>
+        <v>590.1697257198557</v>
       </c>
       <c r="Z36" t="n">
         <v>631.6937413427192</v>
@@ -4324,7 +4324,7 @@
         <v>119.0682906178812</v>
       </c>
       <c r="AC36" t="n">
-        <v>125.891060546875</v>
+        <v>111.2414067401095</v>
       </c>
       <c r="AD36" t="inlineStr">
         <is>
@@ -4410,7 +4410,7 @@
         <v>152.4799242783063</v>
       </c>
       <c r="V37" t="n">
-        <v>192.3937540660137</v>
+        <v>149.4562851418366</v>
       </c>
       <c r="W37" t="n">
         <v>152.4799258306665</v>
@@ -4419,7 +4419,7 @@
         <v>811.982947051163</v>
       </c>
       <c r="Y37" t="n">
-        <v>1024.53125</v>
+        <v>795.8815263003974</v>
       </c>
       <c r="Z37" t="n">
         <v>811.9829553177594</v>
@@ -4431,7 +4431,7 @@
         <v>153.051100830976</v>
       </c>
       <c r="AC37" t="n">
-        <v>193.1144423922937</v>
+        <v>150.0161338776429</v>
       </c>
       <c r="AD37" t="inlineStr">
         <is>
@@ -4517,7 +4517,7 @@
         <v>160.4801055532219</v>
       </c>
       <c r="V38" t="n">
-        <v>137.5980646168326</v>
+        <v>143.9453970158842</v>
       </c>
       <c r="W38" t="n">
         <v>160.4801011700442</v>
@@ -4526,7 +4526,7 @@
         <v>854.5853473297266</v>
       </c>
       <c r="Y38" t="n">
-        <v>732.734375</v>
+        <v>766.5350585436796</v>
       </c>
       <c r="Z38" t="n">
         <v>854.5853239885195</v>
@@ -4538,7 +4538,7 @@
         <v>161.0812440505651</v>
       </c>
       <c r="AC38" t="n">
-        <v>138.1134936096784</v>
+        <v>144.4846024997352</v>
       </c>
       <c r="AD38" t="inlineStr">
         <is>
@@ -4624,7 +4624,7 @@
         <v>119.4424949382637</v>
       </c>
       <c r="V39" t="n">
-        <v>105.9383329350835</v>
+        <v>100.5152574056096</v>
       </c>
       <c r="W39" t="n">
         <v>119.4425248700071</v>
@@ -4633,7 +4633,7 @@
         <v>636.0527099036168</v>
       </c>
       <c r="Y39" t="n">
-        <v>564.140625</v>
+        <v>535.2617750704439</v>
       </c>
       <c r="Z39" t="n">
         <v>636.0528692955191</v>
@@ -4645,7 +4645,7 @@
         <v>119.8899449733941</v>
       </c>
       <c r="AC39" t="n">
-        <v>106.3351676463896</v>
+        <v>100.8917778024225</v>
       </c>
       <c r="AD39" t="inlineStr">
         <is>
@@ -4731,7 +4731,7 @@
         <v>139.2319610626539</v>
       </c>
       <c r="V40" t="n">
-        <v>129.0742907025156</v>
+        <v>126.679122586973</v>
       </c>
       <c r="W40" t="n">
         <v>139.2319544227588</v>
@@ -4740,7 +4740,7 @@
         <v>741.4351666454161</v>
       </c>
       <c r="Y40" t="n">
-        <v>687.34375</v>
+        <v>674.5890501642925</v>
       </c>
       <c r="Z40" t="n">
         <v>741.4351312867839</v>
@@ -4752,7 +4752,7 @@
         <v>139.7535038082092</v>
       </c>
       <c r="AC40" t="n">
-        <v>129.557790465716</v>
+        <v>127.1536502829215</v>
       </c>
       <c r="AD40" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
         <v>172.5277916064204</v>
       </c>
       <c r="V41" t="n">
-        <v>142.4687925678709</v>
+        <v>164.928113212401</v>
       </c>
       <c r="W41" t="n">
         <v>172.5277845472153</v>
@@ -4847,7 +4847,7 @@
         <v>918.7414365521234</v>
       </c>
       <c r="Y41" t="n">
-        <v>758.671875</v>
+        <v>878.2717859523898</v>
       </c>
       <c r="Z41" t="n">
         <v>918.7413989605902</v>
@@ -4859,7 +4859,7 @@
         <v>173.1740568801491</v>
       </c>
       <c r="AC41" t="n">
-        <v>143.0024668347998</v>
+        <v>165.5459179142458</v>
       </c>
       <c r="AD41" t="inlineStr">
         <is>
@@ -4945,7 +4945,7 @@
         <v>147.4310698131381</v>
       </c>
       <c r="V42" t="n">
-        <v>178.9992522006584</v>
+        <v>140.5643479812306</v>
       </c>
       <c r="W42" t="n">
         <v>147.5250647667818</v>
@@ -4954,7 +4954,7 @@
         <v>785.0968914129326</v>
       </c>
       <c r="Y42" t="n">
-        <v>953.203125</v>
+        <v>748.5303659765998</v>
       </c>
       <c r="Z42" t="n">
         <v>785.597431400926</v>
@@ -4966,7 +4966,7 @@
         <v>148.0776793385346</v>
       </c>
       <c r="AC42" t="n">
-        <v>179.6697660232099</v>
+        <v>141.0908883836101</v>
       </c>
       <c r="AD42" t="inlineStr">
         <is>
@@ -5052,7 +5052,7 @@
         <v>158.27608948495</v>
       </c>
       <c r="V43" t="n">
-        <v>120.5505167881985</v>
+        <v>148.5047810309958</v>
       </c>
       <c r="W43" t="n">
         <v>158.2760865955052</v>
@@ -5061,7 +5061,7 @@
         <v>842.8485664326093</v>
       </c>
       <c r="Y43" t="n">
-        <v>641.953125</v>
+        <v>790.8145962392197</v>
       </c>
       <c r="Z43" t="n">
         <v>842.8485510457975</v>
@@ -5073,7 +5073,7 @@
         <v>158.8689734513827</v>
       </c>
       <c r="AC43" t="n">
-        <v>121.0020873217536</v>
+        <v>149.0610655247693</v>
       </c>
       <c r="AD43" t="inlineStr">
         <is>
@@ -5159,7 +5159,7 @@
         <v>122.4260412324264</v>
       </c>
       <c r="V44" t="n">
-        <v>135.1627006413134</v>
+        <v>109.3538629453479</v>
       </c>
       <c r="W44" t="n">
         <v>122.4260353007626</v>
@@ -5168,7 +5168,7 @@
         <v>651.9406290776586</v>
       </c>
       <c r="Y44" t="n">
-        <v>719.765625</v>
+        <v>582.3289349470473</v>
       </c>
       <c r="Z44" t="n">
         <v>651.9405974904848</v>
@@ -5180,7 +5180,7 @@
         <v>122.8846313446015</v>
       </c>
       <c r="AC44" t="n">
-        <v>135.6690069971177</v>
+        <v>109.7634919005128</v>
       </c>
       <c r="AD44" t="inlineStr">
         <is>
@@ -5266,7 +5266,7 @@
         <v>145.7062345154444</v>
       </c>
       <c r="V45" t="n">
-        <v>135.1627006413134</v>
+        <v>134.9675463389499</v>
       </c>
       <c r="W45" t="n">
         <v>145.7062615500503</v>
@@ -5275,7 +5275,7 @@
         <v>775.9118340696264</v>
       </c>
       <c r="Y45" t="n">
-        <v>719.765625</v>
+        <v>718.7263933351568</v>
       </c>
       <c r="Z45" t="n">
         <v>775.911978033752</v>
@@ -5287,7 +5287,7 @@
         <v>146.2520630615119</v>
       </c>
       <c r="AC45" t="n">
-        <v>135.6690069971177</v>
+        <v>135.4731216656819</v>
       </c>
       <c r="AD45" t="inlineStr">
         <is>
@@ -5373,7 +5373,7 @@
         <v>158.1850441785413</v>
       </c>
       <c r="V46" t="n">
-        <v>204.5705739436096</v>
+        <v>156.0132407271587</v>
       </c>
       <c r="W46" t="n">
         <v>158.1850472503425</v>
@@ -5382,7 +5382,7 @@
         <v>842.3637338452188</v>
       </c>
       <c r="Y46" t="n">
-        <v>1089.375</v>
+        <v>830.798490911003</v>
       </c>
       <c r="Z46" t="n">
         <v>842.3637502031114</v>
@@ -5394,7 +5394,7 @@
         <v>158.7775930816705</v>
       </c>
       <c r="AC46" t="n">
-        <v>205.3368754550971</v>
+        <v>156.5976511820771</v>
       </c>
       <c r="AD46" t="inlineStr">
         <is>
@@ -5480,7 +5480,7 @@
         <v>138.4603255233197</v>
       </c>
       <c r="V47" t="n">
-        <v>163.1693863597838</v>
+        <v>125.3260165936287</v>
       </c>
       <c r="W47" t="n">
         <v>138.4603266200077</v>
@@ -5489,7 +5489,7 @@
         <v>737.3260689904721</v>
       </c>
       <c r="Y47" t="n">
-        <v>868.90625</v>
+        <v>667.3835180435984</v>
       </c>
       <c r="Z47" t="n">
         <v>737.3260748305325</v>
@@ -5501,7 +5501,7 @@
         <v>138.978985562614</v>
       </c>
       <c r="AC47" t="n">
-        <v>163.7806030415655</v>
+        <v>125.7954756858776</v>
       </c>
       <c r="AD47" t="inlineStr">
         <is>
@@ -5587,7 +5587,7 @@
         <v>138.9141346290938</v>
       </c>
       <c r="V48" t="n">
-        <v>180.216934188418</v>
+        <v>133.8208017725088</v>
       </c>
       <c r="W48" t="n">
         <v>138.9141517008288</v>
@@ -5596,7 +5596,7 @@
         <v>739.7426838782958</v>
       </c>
       <c r="Y48" t="n">
-        <v>959.6875</v>
+        <v>712.6197728276979</v>
       </c>
       <c r="Z48" t="n">
         <v>739.7427747883465</v>
@@ -5608,7 +5608,7 @@
         <v>139.4345106281332</v>
       </c>
       <c r="AC48" t="n">
-        <v>180.8920093294903</v>
+        <v>134.3220815054142</v>
       </c>
       <c r="AD48" t="inlineStr">
         <is>
@@ -5694,7 +5694,7 @@
         <v>123.6587992973366</v>
       </c>
       <c r="V49" t="n">
-        <v>96.19687703300687</v>
+        <v>115.7232480753053</v>
       </c>
       <c r="W49" t="n">
         <v>123.6587948116768</v>
@@ -5703,7 +5703,7 @@
         <v>658.5052868926763</v>
       </c>
       <c r="Y49" t="n">
-        <v>512.265625</v>
+        <v>616.2470532383908</v>
       </c>
       <c r="Z49" t="n">
         <v>658.5052630057334</v>
@@ -5715,7 +5715,7 @@
         <v>124.1220086529746</v>
       </c>
       <c r="AC49" t="n">
-        <v>96.55722119614686</v>
+        <v>116.1567361288648</v>
       </c>
       <c r="AD49" t="inlineStr">
         <is>
@@ -5801,7 +5801,7 @@
         <v>96.36795249673628</v>
       </c>
       <c r="V50" t="n">
-        <v>113.244424861641</v>
+        <v>91.75567240425681</v>
       </c>
       <c r="W50" t="n">
         <v>96.36796488922003</v>
@@ -5810,7 +5810,7 @@
         <v>513.1766325301035</v>
       </c>
       <c r="Y50" t="n">
-        <v>603.046875</v>
+        <v>488.6154137346288</v>
       </c>
       <c r="Z50" t="n">
         <v>513.1766985223023</v>
@@ -5822,7 +5822,7 @@
         <v>96.72894993086118</v>
       </c>
       <c r="AC50" t="n">
-        <v>113.6686274840716</v>
+        <v>92.09938024598344</v>
       </c>
       <c r="AD50" t="inlineStr">
         <is>
@@ -5908,7 +5908,7 @@
         <v>166.1877603330804</v>
       </c>
       <c r="V51" t="n">
-        <v>113.244424861641</v>
+        <v>133.9333992494458</v>
       </c>
       <c r="W51" t="n">
         <v>166.1877816037669</v>
@@ -5917,7 +5917,7 @@
         <v>884.9796328124585</v>
       </c>
       <c r="Y51" t="n">
-        <v>603.046875</v>
+        <v>713.2193745889564</v>
       </c>
       <c r="Z51" t="n">
         <v>884.9797460826793</v>
@@ -5929,7 +5929,7 @@
         <v>166.8103049011245</v>
       </c>
       <c r="AC51" t="n">
-        <v>113.6686274840716</v>
+        <v>134.4351007615695</v>
       </c>
       <c r="AD51" t="inlineStr">
         <is>
@@ -6015,7 +6015,7 @@
         <v>128.282798228615</v>
       </c>
       <c r="V52" t="n">
-        <v>110.8090608861218</v>
+        <v>115.3309391323641</v>
       </c>
       <c r="W52" t="n">
         <v>128.282806079304</v>
@@ -6024,7 +6024,7 @@
         <v>683.128910606759</v>
       </c>
       <c r="Y52" t="n">
-        <v>590.078125</v>
+        <v>614.1579377489149</v>
       </c>
       <c r="Z52" t="n">
         <v>683.1289524130859</v>
@@ -6036,7 +6036,7 @@
         <v>128.7633410179385</v>
       </c>
       <c r="AC52" t="n">
-        <v>111.2241408715109</v>
+        <v>115.7629576347063</v>
       </c>
       <c r="AD52" t="inlineStr">
         <is>
@@ -6122,7 +6122,7 @@
         <v>169.5358709360638</v>
       </c>
       <c r="V53" t="n">
-        <v>121.7681987759581</v>
+        <v>110.6468593319974</v>
       </c>
       <c r="W53" t="n">
         <v>169.5358441687618</v>
@@ -6131,7 +6131,7 @@
         <v>902.8089223227398</v>
       </c>
       <c r="Y53" t="n">
-        <v>648.4375</v>
+        <v>589.2143726302529</v>
       </c>
       <c r="Z53" t="n">
         <v>902.8087797820552</v>
@@ -6143,7 +6143,7 @@
         <v>170.1709089834777</v>
       </c>
       <c r="AC53" t="n">
-        <v>122.224330628034</v>
+        <v>111.0613317261103</v>
       </c>
       <c r="AD53" t="inlineStr">
         <is>
@@ -6229,7 +6229,7 @@
         <v>150.6526420559427</v>
       </c>
       <c r="V54" t="n">
-        <v>97.41455902076645</v>
+        <v>120.0275454120225</v>
       </c>
       <c r="W54" t="n">
         <v>150.6526784838332</v>
@@ -6238,7 +6238,7 @@
         <v>802.2523414581214</v>
       </c>
       <c r="Y54" t="n">
-        <v>518.75</v>
+        <v>639.1682086166754</v>
       </c>
       <c r="Z54" t="n">
         <v>802.2525354431725</v>
@@ -6250,7 +6250,7 @@
         <v>151.2170087929598</v>
       </c>
       <c r="AC54" t="n">
-        <v>97.77946450242719</v>
+        <v>120.4771569455695</v>
       </c>
       <c r="AD54" t="inlineStr">
         <is>
@@ -6336,7 +6336,7 @@
         <v>102.0519678535106</v>
       </c>
       <c r="V55" t="n">
-        <v>58.44873541245988</v>
+        <v>75.2293353344853</v>
       </c>
       <c r="W55" t="n">
         <v>102.0519681292183</v>
@@ -6345,7 +6345,7 @@
         <v>543.4450338447174</v>
       </c>
       <c r="Y55" t="n">
-        <v>311.25</v>
+        <v>400.6097045149587</v>
       </c>
       <c r="Z55" t="n">
         <v>543.44503531291</v>
@@ -6357,7 +6357,7 @@
         <v>102.4342448952269</v>
       </c>
       <c r="AC55" t="n">
-        <v>58.66767870145632</v>
+        <v>75.51113712182794</v>
       </c>
       <c r="AD55" t="inlineStr">
         <is>
@@ -6443,7 +6443,7 @@
         <v>153.7109530585857</v>
       </c>
       <c r="V56" t="n">
-        <v>202.1352099680904</v>
+        <v>147.1640940312401</v>
       </c>
       <c r="W56" t="n">
         <v>153.7109447850978</v>
@@ -6452,7 +6452,7 @@
         <v>818.53839611534</v>
       </c>
       <c r="Y56" t="n">
-        <v>1076.40625</v>
+        <v>783.6751974869755</v>
       </c>
       <c r="Z56" t="n">
         <v>818.5383520575333</v>
@@ -6464,7 +6464,7 @@
         <v>154.2867310629105</v>
       </c>
       <c r="AC56" t="n">
-        <v>202.8923888425364</v>
+        <v>147.7153564416585</v>
       </c>
       <c r="AD56" t="inlineStr">
         <is>
@@ -6550,28 +6550,28 @@
         <v>151.4488057950835</v>
       </c>
       <c r="V57" t="n">
-        <v>149.7748844944284</v>
+        <v>134.8997502706081</v>
       </c>
       <c r="W57" t="n">
-        <v>151.4513975732121</v>
+        <v>151.4513975732123</v>
       </c>
       <c r="X57" t="n">
         <v>806.4920561766497</v>
       </c>
       <c r="Y57" t="n">
-        <v>797.578125</v>
+        <v>718.3653671106804</v>
       </c>
       <c r="Z57" t="n">
-        <v>806.5058578600709</v>
+        <v>806.5058578600721</v>
       </c>
       <c r="AA57" t="n">
         <v>152.0161183198347</v>
       </c>
       <c r="AB57" t="n">
-        <v>152.0187198065126</v>
+        <v>152.0187198065128</v>
       </c>
       <c r="AC57" t="n">
-        <v>150.3359266724818</v>
+        <v>135.4050716398494</v>
       </c>
       <c r="AD57" t="inlineStr">
         <is>
@@ -6657,7 +6657,7 @@
         <v>128.4136371924826</v>
       </c>
       <c r="V58" t="n">
-        <v>105.9383329350835</v>
+        <v>117.1573194811519</v>
       </c>
       <c r="W58" t="n">
         <v>128.4136733627494</v>
@@ -6666,7 +6666,7 @@
         <v>683.8256515578918</v>
       </c>
       <c r="Y58" t="n">
-        <v>564.140625</v>
+        <v>623.8837407033963</v>
       </c>
       <c r="Z58" t="n">
         <v>683.8258441710507</v>
@@ -6678,7 +6678,7 @@
         <v>128.894698517524</v>
       </c>
       <c r="AC58" t="n">
-        <v>106.3351676463896</v>
+        <v>117.5961794269865</v>
       </c>
       <c r="AD58" t="inlineStr">
         <is>
@@ -6764,7 +6764,7 @@
         <v>132.1131426406206</v>
       </c>
       <c r="V59" t="n">
-        <v>137.5980646168326</v>
+        <v>120.491413973953</v>
       </c>
       <c r="W59" t="n">
         <v>132.1164615225414</v>
@@ -6773,7 +6773,7 @@
         <v>703.5261816481888</v>
       </c>
       <c r="Y59" t="n">
-        <v>732.734375</v>
+        <v>641.6383919128922</v>
       </c>
       <c r="Z59" t="n">
         <v>703.5438552897234</v>
@@ -6785,7 +6785,7 @@
         <v>132.6113569623176</v>
       </c>
       <c r="AC59" t="n">
-        <v>138.1134936096784</v>
+        <v>120.9427631141033</v>
       </c>
       <c r="AD59" t="inlineStr">
         <is>
@@ -6871,7 +6871,7 @@
         <v>134.0967986485918</v>
       </c>
       <c r="V60" t="n">
-        <v>174.12852424962</v>
+        <v>129.9771983471983</v>
       </c>
       <c r="W60" t="n">
         <v>134.0967931066156</v>
@@ -6880,7 +6880,7 @@
         <v>714.0895056982999</v>
       </c>
       <c r="Y60" t="n">
-        <v>927.265625</v>
+        <v>692.1518951621549</v>
       </c>
       <c r="Z60" t="n">
         <v>714.0894761862829</v>
@@ -6892,7 +6892,7 @@
         <v>134.5991066762669</v>
       </c>
       <c r="AC60" t="n">
-        <v>174.7807927980886</v>
+        <v>130.4640803147868</v>
       </c>
       <c r="AD60" t="inlineStr">
         <is>
@@ -6978,7 +6978,7 @@
         <v>148.6912733137501</v>
       </c>
       <c r="V61" t="n">
-        <v>191.1760720782542</v>
+        <v>138.0784969123962</v>
       </c>
       <c r="W61" t="n">
         <v>148.6912866347793</v>
@@ -6987,7 +6987,7 @@
         <v>791.80770109594</v>
       </c>
       <c r="Y61" t="n">
-        <v>1018.046875</v>
+        <v>735.2927631488444</v>
       </c>
       <c r="Z61" t="n">
         <v>791.8077720328102</v>
@@ -6999,7 +6999,7 @@
         <v>149.2482697604398</v>
       </c>
       <c r="AC61" t="n">
-        <v>191.8921990860134</v>
+        <v>138.5957255579837</v>
       </c>
       <c r="AD61" t="inlineStr">
         <is>
@@ -7085,7 +7085,7 @@
         <v>139.9372559195478</v>
       </c>
       <c r="V62" t="n">
-        <v>97.41455902076645</v>
+        <v>123.0907255124977</v>
       </c>
       <c r="W62" t="n">
         <v>139.9372601068099</v>
@@ -7094,7 +7094,7 @@
         <v>745.1909882668612</v>
       </c>
       <c r="Y62" t="n">
-        <v>518.75</v>
+        <v>655.4801920932184</v>
       </c>
       <c r="Z62" t="n">
         <v>745.1910105647829</v>
@@ -7106,7 +7106,7 @@
         <v>140.4614514988859</v>
       </c>
       <c r="AC62" t="n">
-        <v>97.77946450242719</v>
+        <v>123.5518114213456</v>
       </c>
       <c r="AD62" t="inlineStr">
         <is>
@@ -7192,7 +7192,7 @@
         <v>112.8503285653132</v>
       </c>
       <c r="V63" t="n">
-        <v>60.88409938797903</v>
+        <v>74.09656429725177</v>
       </c>
       <c r="W63" t="n">
         <v>112.850341470895</v>
@@ -7201,7 +7201,7 @@
         <v>600.9482415331438</v>
       </c>
       <c r="Y63" t="n">
-        <v>324.21875</v>
+        <v>394.5774955569565</v>
       </c>
       <c r="Z63" t="n">
         <v>600.9483102576817</v>
@@ -7213,7 +7213,7 @@
         <v>113.2730678951992</v>
       </c>
       <c r="AC63" t="n">
-        <v>61.11216531401699</v>
+        <v>74.37412283425166</v>
       </c>
       <c r="AD63" t="inlineStr">
         <is>
@@ -7299,7 +7299,7 @@
         <v>155.1349261705808</v>
       </c>
       <c r="V64" t="n">
-        <v>178.9992522006584</v>
+        <v>143.1672248336066</v>
       </c>
       <c r="W64" t="n">
         <v>155.1349103138343</v>
@@ -7308,7 +7308,7 @@
         <v>826.1213083542591</v>
       </c>
       <c r="Y64" t="n">
-        <v>953.203125</v>
+        <v>762.391152092587</v>
       </c>
       <c r="Z64" t="n">
         <v>826.1212239142401</v>
@@ -7320,7 +7320,7 @@
         <v>155.7160306282875</v>
       </c>
       <c r="AC64" t="n">
-        <v>179.6697660232099</v>
+        <v>143.7035153600033</v>
       </c>
       <c r="AD64" t="inlineStr">
         <is>
@@ -7406,19 +7406,19 @@
         <v>154.7858780452867</v>
       </c>
       <c r="V65" t="n">
-        <v>183.8699801516967</v>
+        <v>145.6748989141434</v>
       </c>
       <c r="W65" t="n">
-        <v>155.2819605154789</v>
+        <v>155.2819605154788</v>
       </c>
       <c r="X65" t="n">
         <v>824.2625644784316</v>
       </c>
       <c r="Y65" t="n">
-        <v>979.140625</v>
+        <v>775.7449663720431</v>
       </c>
       <c r="Z65" t="n">
-        <v>826.9042926143389</v>
+        <v>826.9042926143387</v>
       </c>
       <c r="AA65" t="n">
         <v>155.3656909187439</v>
@@ -7427,7 +7427,7 @@
         <v>155.8636316657126</v>
       </c>
       <c r="AC65" t="n">
-        <v>184.5587392483313</v>
+        <v>146.2205829442155</v>
       </c>
       <c r="AD65" t="inlineStr">
         <is>
@@ -7513,28 +7513,28 @@
         <v>128.0406726662717</v>
       </c>
       <c r="V66" t="n">
-        <v>175.3462062373796</v>
+        <v>126.2588893153503</v>
       </c>
       <c r="W66" t="n">
-        <v>128.040682502547</v>
+        <v>128.0406825025471</v>
       </c>
       <c r="X66" t="n">
         <v>681.8395485573058</v>
       </c>
       <c r="Y66" t="n">
-        <v>933.75</v>
+        <v>672.3512326158107</v>
       </c>
       <c r="Z66" t="n">
-        <v>681.8396009372365</v>
+        <v>681.8396009372368</v>
       </c>
       <c r="AA66" t="n">
         <v>128.5203005966459</v>
       </c>
       <c r="AB66" t="n">
-        <v>128.520310469767</v>
+        <v>128.5203104697671</v>
       </c>
       <c r="AC66" t="n">
-        <v>176.0030361043689</v>
+        <v>126.731842858257</v>
       </c>
       <c r="AD66" t="inlineStr">
         <is>
@@ -7620,7 +7620,7 @@
         <v>127.8649067072094</v>
       </c>
       <c r="V67" t="n">
-        <v>166.8224323230625</v>
+        <v>120.6066597640275</v>
       </c>
       <c r="W67" t="n">
         <v>127.8649118766067</v>
@@ -7629,7 +7629,7 @@
         <v>680.9035632982227</v>
       </c>
       <c r="Y67" t="n">
-        <v>888.359375</v>
+        <v>642.2520964166349</v>
       </c>
       <c r="Z67" t="n">
         <v>680.9035908261903</v>
@@ -7641,7 +7641,7 @@
         <v>128.3438814241247</v>
       </c>
       <c r="AC67" t="n">
-        <v>167.4473329604066</v>
+        <v>121.0584406037201</v>
       </c>
       <c r="AD67" t="inlineStr">
         <is>
@@ -7727,7 +7727,7 @@
         <v>137.5223119684616</v>
       </c>
       <c r="V68" t="n">
-        <v>154.6456124454668</v>
+        <v>126.1175473065487</v>
       </c>
       <c r="W68" t="n">
         <v>137.5223104096348</v>
@@ -7736,7 +7736,7 @@
         <v>732.3309785596989</v>
       </c>
       <c r="Y68" t="n">
-        <v>823.515625</v>
+        <v>671.5985610664769</v>
       </c>
       <c r="Z68" t="n">
         <v>732.3309702586666</v>
@@ -7748,7 +7748,7 @@
         <v>138.0374556345742</v>
       </c>
       <c r="AC68" t="n">
-        <v>155.2248998976032</v>
+        <v>126.5899713960111</v>
       </c>
       <c r="AD68" t="inlineStr">
         <is>
@@ -7834,19 +7834,19 @@
         <v>142.2383720902759</v>
       </c>
       <c r="V69" t="n">
-        <v>175.3462062373796</v>
+        <v>127.6272003643167</v>
       </c>
       <c r="W69" t="n">
-        <v>142.2391787457396</v>
+        <v>142.2391787457397</v>
       </c>
       <c r="X69" t="n">
         <v>757.4448446263683</v>
       </c>
       <c r="Y69" t="n">
-        <v>933.75</v>
+        <v>679.6377343850179</v>
       </c>
       <c r="Z69" t="n">
-        <v>757.4491402114019</v>
+        <v>757.4491402114023</v>
       </c>
       <c r="AA69" t="n">
         <v>142.7711832244635</v>
@@ -7855,7 +7855,7 @@
         <v>142.7719929015803</v>
       </c>
       <c r="AC69" t="n">
-        <v>176.0030361043689</v>
+        <v>128.1052794675853</v>
       </c>
       <c r="AD69" t="inlineStr">
         <is>
@@ -7941,7 +7941,7 @@
         <v>151.1171136528311</v>
       </c>
       <c r="V70" t="n">
-        <v>198.4821640048116</v>
+        <v>147.3349073440194</v>
       </c>
       <c r="W70" t="n">
         <v>151.1171114806128</v>
@@ -7950,7 +7950,7 @@
         <v>804.7257360236555</v>
       </c>
       <c r="Y70" t="n">
-        <v>1056.953125</v>
+        <v>784.584809016248</v>
       </c>
       <c r="Z70" t="n">
         <v>804.7257244562038</v>
@@ -7962,7 +7962,7 @@
         <v>151.683181510661</v>
       </c>
       <c r="AC70" t="n">
-        <v>199.2256589236954</v>
+        <v>147.886809604526</v>
       </c>
       <c r="AD70" t="inlineStr">
         <is>
@@ -8048,7 +8048,7 @@
         <v>160.6682516331869</v>
       </c>
       <c r="V71" t="n">
-        <v>193.6114360537733</v>
+        <v>153.3497314802519</v>
       </c>
       <c r="W71" t="n">
         <v>160.6682393357454</v>
@@ -8057,7 +8057,7 @@
         <v>855.5872589532352</v>
       </c>
       <c r="Y71" t="n">
-        <v>1031.015625</v>
+        <v>816.6148264185282</v>
       </c>
       <c r="Z71" t="n">
         <v>855.5871934671532</v>
@@ -8069,7 +8069,7 @@
         <v>161.2700869635717</v>
       </c>
       <c r="AC71" t="n">
-        <v>194.3366856985741</v>
+        <v>153.9241646880891</v>
       </c>
       <c r="AD71" t="inlineStr">
         <is>
@@ -8155,7 +8155,7 @@
         <v>143.9960367554822</v>
       </c>
       <c r="V72" t="n">
-        <v>94.97919504524729</v>
+        <v>118.5080041052441</v>
       </c>
       <c r="W72" t="n">
         <v>143.9960184935385</v>
@@ -8164,7 +8164,7 @@
         <v>766.8047242402704</v>
       </c>
       <c r="Y72" t="n">
-        <v>505.78125</v>
+        <v>631.0763785985023</v>
       </c>
       <c r="Z72" t="n">
         <v>766.804626992145</v>
@@ -8176,7 +8176,7 @@
         <v>144.5354136005308</v>
       </c>
       <c r="AC72" t="n">
-        <v>95.33497788986651</v>
+        <v>118.951923584564</v>
       </c>
       <c r="AD72" t="inlineStr">
         <is>
@@ -8262,28 +8262,28 @@
         <v>136.1843117549759</v>
       </c>
       <c r="V73" t="n">
-        <v>127.856608714756</v>
+        <v>124.7332851746996</v>
       </c>
       <c r="W73" t="n">
-        <v>136.197274245338</v>
+        <v>136.1972742453382</v>
       </c>
       <c r="X73" t="n">
         <v>725.2058874262708</v>
       </c>
       <c r="Y73" t="n">
-        <v>680.859375</v>
+        <v>664.2271169197797</v>
       </c>
       <c r="Z73" t="n">
-        <v>725.2749150125262</v>
+        <v>725.2749150125272</v>
       </c>
       <c r="AA73" t="n">
         <v>136.69444496684</v>
       </c>
       <c r="AB73" t="n">
-        <v>136.7074560134327</v>
+        <v>136.7074560134329</v>
       </c>
       <c r="AC73" t="n">
-        <v>128.3355471594357</v>
+        <v>125.2005239525921</v>
       </c>
       <c r="AD73" t="inlineStr">
         <is>
@@ -8369,7 +8369,7 @@
         <v>123.2664893679007</v>
       </c>
       <c r="V74" t="n">
-        <v>140.0334285923518</v>
+        <v>115.3859311676189</v>
       </c>
       <c r="W74" t="n">
         <v>123.2664907229534</v>
@@ -8378,7 +8378,7 @@
         <v>656.4161661499392</v>
       </c>
       <c r="Y74" t="n">
-        <v>745.703125</v>
+        <v>614.4507802005483</v>
       </c>
       <c r="Z74" t="n">
         <v>656.4161733658381</v>
@@ -8390,7 +8390,7 @@
         <v>123.7282350312175</v>
       </c>
       <c r="AC74" t="n">
-        <v>140.5579802222391</v>
+        <v>115.8181556647869</v>
       </c>
       <c r="AD74" t="inlineStr">
         <is>
@@ -8476,28 +8476,28 @@
         <v>133.9093135460643</v>
       </c>
       <c r="V75" t="n">
-        <v>149.7748844944284</v>
+        <v>122.2897305109332</v>
       </c>
       <c r="W75" t="n">
-        <v>133.9148791591712</v>
+        <v>133.9148791591713</v>
       </c>
       <c r="X75" t="n">
         <v>713.0911138982055</v>
       </c>
       <c r="Y75" t="n">
-        <v>797.578125</v>
+        <v>651.2147500357024</v>
       </c>
       <c r="Z75" t="n">
-        <v>713.1207517863018</v>
+        <v>713.1207517863028</v>
       </c>
       <c r="AA75" t="n">
         <v>134.4109248354812</v>
       </c>
       <c r="AB75" t="n">
-        <v>134.4165112968345</v>
+        <v>134.4165112968347</v>
       </c>
       <c r="AC75" t="n">
-        <v>150.3359266724818</v>
+        <v>122.7478159702611</v>
       </c>
       <c r="AD75" t="inlineStr">
         <is>
@@ -8583,7 +8583,7 @@
         <v>99.92224303699318</v>
       </c>
       <c r="V76" t="n">
-        <v>98.35123747288921</v>
+        <v>87.87514035515903</v>
       </c>
       <c r="W76" t="n">
         <v>99.92388500113036</v>
@@ -8592,7 +8592,7 @@
         <v>494.096448103874</v>
       </c>
       <c r="Y76" t="n">
-        <v>486.328125</v>
+        <v>434.5258213432918</v>
       </c>
       <c r="Z76" t="n">
         <v>494.1045673035982</v>
@@ -8604,7 +8604,7 @@
         <v>100.298190174323</v>
       </c>
       <c r="AC76" t="n">
-        <v>98.71965166110436</v>
+        <v>88.20431210052891</v>
       </c>
       <c r="AD76" t="inlineStr">
         <is>
@@ -8690,7 +8690,7 @@
         <v>93.16987866025877</v>
       </c>
       <c r="V77" t="n">
-        <v>95.72853780694551</v>
+        <v>82.48950412206295</v>
       </c>
       <c r="W77" t="n">
         <v>93.16986909818462</v>
@@ -8699,7 +8699,7 @@
         <v>460.707293162542</v>
       </c>
       <c r="Y77" t="n">
-        <v>473.359375</v>
+        <v>407.8948765939116</v>
       </c>
       <c r="Z77" t="n">
         <v>460.7072458799078</v>
@@ -8711,7 +8711,7 @@
         <v>93.51887438344484</v>
       </c>
       <c r="AC77" t="n">
-        <v>96.08712761680826</v>
+        <v>82.79850179690948</v>
       </c>
       <c r="AD77" t="inlineStr">
         <is>
@@ -8797,7 +8797,7 @@
         <v>110.0196575904515</v>
       </c>
       <c r="V78" t="n">
-        <v>137.6917324620449</v>
+        <v>101.1635607966164</v>
       </c>
       <c r="W78" t="n">
         <v>110.0206113276522</v>
@@ -8806,7 +8806,7 @@
         <v>544.0262386516007</v>
       </c>
       <c r="Y78" t="n">
-        <v>680.859375</v>
+        <v>500.2345278482509</v>
       </c>
       <c r="Z78" t="n">
         <v>544.0309547002901</v>
@@ -8818,7 +8818,7 @@
         <v>110.4327378575333</v>
       </c>
       <c r="AC78" t="n">
-        <v>138.2075123255461</v>
+        <v>101.5425096749984</v>
       </c>
       <c r="AD78" t="inlineStr">
         <is>
@@ -8904,7 +8904,7 @@
         <v>75.30618550066463</v>
       </c>
       <c r="V79" t="n">
-        <v>86.54908897614251</v>
+        <v>73.41168272055538</v>
       </c>
       <c r="W79" t="n">
         <v>75.30617977808573</v>
@@ -8913,7 +8913,7 @@
         <v>372.3747350462752</v>
       </c>
       <c r="Y79" t="n">
-        <v>427.96875</v>
+        <v>363.0067798630799</v>
       </c>
       <c r="Z79" t="n">
         <v>372.3747067492133</v>
@@ -8925,7 +8925,7 @@
         <v>75.58826941725451</v>
       </c>
       <c r="AC79" t="n">
-        <v>86.87329346177184</v>
+        <v>73.68667575765323</v>
       </c>
       <c r="AD79" t="inlineStr">
         <is>
@@ -9011,7 +9011,7 @@
         <v>155.632536619942</v>
       </c>
       <c r="V80" t="n">
-        <v>113.244424861641</v>
+        <v>138.2100790573799</v>
       </c>
       <c r="W80" t="n">
         <v>155.6325250695893</v>
@@ -9020,7 +9020,7 @@
         <v>828.7711732533152</v>
       </c>
       <c r="Y80" t="n">
-        <v>603.046875</v>
+        <v>735.9934616727244</v>
       </c>
       <c r="Z80" t="n">
         <v>828.7711117456154</v>
@@ -9032,7 +9032,7 @@
         <v>156.2155094006121</v>
       </c>
       <c r="AC80" t="n">
-        <v>113.6686274840716</v>
+        <v>138.7278005969092</v>
       </c>
       <c r="AD80" t="inlineStr">
         <is>
@@ -9118,7 +9118,7 @@
         <v>104.0247731660686</v>
       </c>
       <c r="V81" t="n">
-        <v>121.9555344663826</v>
+        <v>87.80798481579551</v>
       </c>
       <c r="W81" t="n">
         <v>104.1011607942594</v>
@@ -9127,7 +9127,7 @@
         <v>514.3826777100772</v>
       </c>
       <c r="Y81" t="n">
-        <v>603.046875</v>
+        <v>434.19375</v>
       </c>
       <c r="Z81" t="n">
         <v>514.7603999731192</v>
@@ -9139,7 +9139,7 @@
         <v>104.4911136370677</v>
       </c>
       <c r="AC81" t="n">
-        <v>122.4123680597694</v>
+        <v>88.13690500303399</v>
       </c>
       <c r="AD81" t="inlineStr">
         <is>
@@ -9225,7 +9225,7 @@
         <v>122.5361790489141</v>
       </c>
       <c r="V82" t="n">
-        <v>161.2960294555383</v>
+        <v>116.1816522044278</v>
       </c>
       <c r="W82" t="n">
         <v>122.5361659874053</v>
@@ -9234,7 +9234,7 @@
         <v>605.9180517982766</v>
       </c>
       <c r="Y82" t="n">
-        <v>797.578125</v>
+        <v>574.4961276319125</v>
       </c>
       <c r="Z82" t="n">
         <v>605.9179872116048</v>
@@ -9246,7 +9246,7 @@
         <v>122.9951745701056</v>
       </c>
       <c r="AC82" t="n">
-        <v>161.9002287242112</v>
+        <v>116.6168573953558</v>
       </c>
       <c r="AD82" t="inlineStr">
         <is>
@@ -9332,7 +9332,7 @@
         <v>76.63952735675873</v>
       </c>
       <c r="V83" t="n">
-        <v>61.63344214967724</v>
+        <v>71.716867548991</v>
       </c>
       <c r="W83" t="n">
         <v>76.6395027019732</v>
@@ -9341,7 +9341,7 @@
         <v>378.9678564092576</v>
       </c>
       <c r="Y83" t="n">
-        <v>304.765625</v>
+        <v>354.6262418466096</v>
       </c>
       <c r="Z83" t="n">
         <v>378.967734496042</v>
@@ -9353,7 +9353,7 @@
         <v>76.9265868393837</v>
       </c>
       <c r="AC83" t="n">
-        <v>61.86431504095874</v>
+        <v>71.98551197297884</v>
       </c>
       <c r="AD83" t="inlineStr">
         <is>
@@ -9439,7 +9439,7 @@
         <v>109.9335361810218</v>
       </c>
       <c r="V84" t="n">
-        <v>115.6797888371602</v>
+        <v>98.71902205402468</v>
       </c>
       <c r="W84" t="n">
         <v>109.9389009866237</v>
@@ -9448,7 +9448,7 @@
         <v>585.4157989027905</v>
       </c>
       <c r="Y84" t="n">
-        <v>616.015625</v>
+        <v>525.6964996331652</v>
       </c>
       <c r="Z84" t="n">
         <v>585.4443674549038</v>
@@ -9460,7 +9460,7 @@
         <v>110.3507214374992</v>
       </c>
       <c r="AC84" t="n">
-        <v>116.1131140966323</v>
+        <v>99.08881392757841</v>
       </c>
       <c r="AD84" t="inlineStr">
         <is>
@@ -9546,19 +9546,19 @@
         <v>139.0069973009075</v>
       </c>
       <c r="V85" t="n">
-        <v>90.10846709420898</v>
+        <v>115.4861820167965</v>
       </c>
       <c r="W85" t="n">
-        <v>139.082277538668</v>
+        <v>139.0822775386679</v>
       </c>
       <c r="X85" t="n">
         <v>740.2371942624477</v>
       </c>
       <c r="Y85" t="n">
-        <v>479.84375</v>
+        <v>614.9846339543777</v>
       </c>
       <c r="Z85" t="n">
-        <v>740.6380750315113</v>
+        <v>740.6380750315111</v>
       </c>
       <c r="AA85" t="n">
         <v>139.527704018817</v>
@@ -9567,7 +9567,7 @@
         <v>139.6032662490403</v>
       </c>
       <c r="AC85" t="n">
-        <v>90.44600466474515</v>
+        <v>115.9187820439137</v>
       </c>
       <c r="AD85" t="inlineStr">
         <is>
@@ -9653,7 +9653,7 @@
         <v>136.2947825283333</v>
       </c>
       <c r="V86" t="n">
-        <v>102.2852869718048</v>
+        <v>120.0046548321027</v>
       </c>
       <c r="W86" t="n">
         <v>136.2947701092442</v>
@@ -9662,7 +9662,7 @@
         <v>725.7941641095018</v>
       </c>
       <c r="Y86" t="n">
-        <v>544.6875</v>
+        <v>639.0463121727271</v>
       </c>
       <c r="Z86" t="n">
         <v>725.7940979756243</v>
@@ -9674,7 +9674,7 @@
         <v>136.8053170873806</v>
       </c>
       <c r="AC86" t="n">
-        <v>102.6684377275486</v>
+        <v>120.4541806197594</v>
       </c>
       <c r="AD86" t="inlineStr">
         <is>
@@ -9760,7 +9760,7 @@
         <v>133.8207995698365</v>
       </c>
       <c r="V87" t="n">
-        <v>163.1693863597838</v>
+        <v>120.7854112625108</v>
       </c>
       <c r="W87" t="n">
         <v>133.8208017725088</v>
@@ -9769,7 +9769,7 @@
         <v>712.6197610980723</v>
       </c>
       <c r="Y87" t="n">
-        <v>868.90625</v>
+        <v>643.2039802086504</v>
       </c>
       <c r="Z87" t="n">
         <v>712.6197728276979</v>
@@ -9781,7 +9781,7 @@
         <v>134.3220815054142</v>
       </c>
       <c r="AC87" t="n">
-        <v>163.7806030415655</v>
+        <v>121.2378616879646</v>
       </c>
       <c r="AD87" t="inlineStr">
         <is>
@@ -9867,28 +9867,28 @@
         <v>143.8053221538262</v>
       </c>
       <c r="V88" t="n">
-        <v>115.6797888371602</v>
+        <v>126.1072760740915</v>
       </c>
       <c r="W88" t="n">
-        <v>143.814467127471</v>
+        <v>143.8144671274709</v>
       </c>
       <c r="X88" t="n">
         <v>765.789134778043</v>
       </c>
       <c r="Y88" t="n">
-        <v>616.015625</v>
+        <v>671.5438649112953</v>
       </c>
       <c r="Z88" t="n">
-        <v>765.8378334030321</v>
+        <v>765.8378334030316</v>
       </c>
       <c r="AA88" t="n">
         <v>144.3440029308416</v>
       </c>
       <c r="AB88" t="n">
-        <v>144.3531821606699</v>
+        <v>144.3531821606698</v>
       </c>
       <c r="AC88" t="n">
-        <v>116.1131140966323</v>
+        <v>126.5796616885142</v>
       </c>
       <c r="AD88" t="inlineStr">
         <is>
@@ -9974,7 +9974,7 @@
         <v>128.6232272953374</v>
       </c>
       <c r="V89" t="n">
-        <v>87.67310311868981</v>
+        <v>107.4991176294036</v>
       </c>
       <c r="W89" t="n">
         <v>128.6232267328338</v>
@@ -9983,7 +9983,7 @@
         <v>684.9417564496953</v>
       </c>
       <c r="Y89" t="n">
-        <v>466.875</v>
+        <v>572.4520834546438</v>
       </c>
       <c r="Z89" t="n">
         <v>684.9417534542627</v>
@@ -9995,7 +9995,7 @@
         <v>129.1050368541905</v>
       </c>
       <c r="AC89" t="n">
-        <v>88.00151805218447</v>
+        <v>107.9017988886628</v>
       </c>
       <c r="AD89" t="inlineStr">
         <is>
@@ -10081,7 +10081,7 @@
         <v>155.1858456411894</v>
       </c>
       <c r="V90" t="n">
-        <v>192.3937540660137</v>
+        <v>146.7083957683407</v>
       </c>
       <c r="W90" t="n">
         <v>155.1857953755431</v>
@@ -10090,7 +10090,7 @@
         <v>826.3924636686571</v>
       </c>
       <c r="Y90" t="n">
-        <v>1024.53125</v>
+        <v>781.2485224986028</v>
       </c>
       <c r="Z90" t="n">
         <v>826.3921959950745</v>
@@ -10102,7 +10102,7 @@
         <v>155.7671063004978</v>
       </c>
       <c r="AC90" t="n">
-        <v>193.1144423922937</v>
+        <v>147.2579511773028</v>
       </c>
       <c r="AD90" t="inlineStr">
         <is>
@@ -10188,7 +10188,7 @@
         <v>134.1714837853786</v>
       </c>
       <c r="V91" t="n">
-        <v>169.2577962985817</v>
+        <v>121.9552858362728</v>
       </c>
       <c r="W91" t="n">
         <v>134.1715019998045</v>
@@ -10197,7 +10197,7 @@
         <v>714.4872174479358</v>
       </c>
       <c r="Y91" t="n">
-        <v>901.328125</v>
+        <v>649.4337721539144</v>
       </c>
       <c r="Z91" t="n">
         <v>714.4873144430211</v>
@@ -10209,7 +10209,7 @@
         <v>134.6740954217174</v>
       </c>
       <c r="AC91" t="n">
-        <v>169.8918195729672</v>
+        <v>122.4121184983153</v>
       </c>
       <c r="AD91" t="inlineStr">
         <is>
@@ -10295,28 +10295,28 @@
         <v>158.2109696797209</v>
       </c>
       <c r="V92" t="n">
-        <v>112.0267428738814</v>
+        <v>137.4396186972558</v>
       </c>
       <c r="W92" t="n">
-        <v>158.2134146233428</v>
+        <v>158.2134146233427</v>
       </c>
       <c r="X92" t="n">
         <v>842.5017917892483</v>
       </c>
       <c r="Y92" t="n">
-        <v>596.5625</v>
+        <v>731.890622057866</v>
       </c>
       <c r="Z92" t="n">
-        <v>842.5148115525834</v>
+        <v>842.5148115525827</v>
       </c>
       <c r="AA92" t="n">
         <v>158.803612613953</v>
       </c>
       <c r="AB92" t="n">
-        <v>158.8060667160963</v>
+        <v>158.8060667160962</v>
       </c>
       <c r="AC92" t="n">
-        <v>112.4463841777913</v>
+        <v>137.9544541670679</v>
       </c>
       <c r="AD92" t="inlineStr">
         <is>
@@ -10402,7 +10402,7 @@
         <v>144.1138129295586</v>
       </c>
       <c r="V93" t="n">
-        <v>102.2852869718048</v>
+        <v>128.0691390838696</v>
       </c>
       <c r="W93" t="n">
         <v>144.1138027337883</v>
@@ -10411,7 +10411,7 @@
         <v>767.4319034926975</v>
       </c>
       <c r="Y93" t="n">
-        <v>544.6875</v>
+        <v>681.9911373370257</v>
       </c>
       <c r="Z93" t="n">
         <v>767.4318491983917</v>
@@ -10423,7 +10423,7 @@
         <v>144.6536390491107</v>
       </c>
       <c r="AC93" t="n">
-        <v>102.6684377275486</v>
+        <v>128.5488736466808</v>
       </c>
       <c r="AD93" t="inlineStr">
         <is>
@@ -10509,7 +10509,7 @@
         <v>107.2063508578886</v>
       </c>
       <c r="V94" t="n">
-        <v>92.54383106972813</v>
+        <v>97.87870520780282</v>
       </c>
       <c r="W94" t="n">
         <v>107.2063487166135</v>
@@ -10518,7 +10518,7 @@
         <v>570.8930478828556</v>
       </c>
       <c r="Y94" t="n">
-        <v>492.8125</v>
+        <v>521.2216616997033</v>
       </c>
       <c r="Z94" t="n">
         <v>570.893036480182</v>
@@ -10530,7 +10530,7 @@
         <v>107.6079332919457</v>
       </c>
       <c r="AC94" t="n">
-        <v>92.89049127730583</v>
+        <v>98.24534933602364</v>
       </c>
       <c r="AD94" t="inlineStr">
         <is>
@@ -10616,7 +10616,7 @@
         <v>159.2682752871106</v>
       </c>
       <c r="V95" t="n">
-        <v>194.8291180415329</v>
+        <v>143.0549963582182</v>
       </c>
       <c r="W95" t="n">
         <v>159.2682757960604</v>
@@ -10625,7 +10625,7 @@
         <v>848.1321337971252</v>
       </c>
       <c r="Y95" t="n">
-        <v>1037.5</v>
+        <v>761.793515330762</v>
       </c>
       <c r="Z95" t="n">
         <v>848.1321365073737</v>
@@ -10637,7 +10637,7 @@
         <v>159.8648792963672</v>
       </c>
       <c r="AC95" t="n">
-        <v>195.5589290048544</v>
+        <v>143.5908664876404</v>
       </c>
       <c r="AD95" t="inlineStr">
         <is>
@@ -10723,7 +10723,7 @@
         <v>185.3783617311769</v>
       </c>
       <c r="V96" t="n">
-        <v>121.7681987759581</v>
+        <v>156.8344146973914</v>
       </c>
       <c r="W96" t="n">
         <v>185.3783445151198</v>
@@ -10732,7 +10732,7 @@
         <v>987.1730274685939</v>
       </c>
       <c r="Y96" t="n">
-        <v>648.4375</v>
+        <v>835.1713895961713</v>
       </c>
       <c r="Z96" t="n">
         <v>987.1729357900016</v>
@@ -10744,7 +10744,7 @@
         <v>186.0727537982367</v>
       </c>
       <c r="AC96" t="n">
-        <v>122.224330628034</v>
+        <v>157.4219011902875</v>
       </c>
       <c r="AD96" t="inlineStr">
         <is>
@@ -10830,7 +10830,7 @@
         <v>141.9683188805451</v>
       </c>
       <c r="V97" t="n">
-        <v>105.9383329350835</v>
+        <v>109.8650103276247</v>
       </c>
       <c r="W97" t="n">
         <v>141.9683100171074</v>
@@ -10839,7 +10839,7 @@
         <v>756.0067628452047</v>
       </c>
       <c r="Y97" t="n">
-        <v>564.140625</v>
+        <v>585.0508864419936</v>
       </c>
       <c r="Z97" t="n">
         <v>756.0067156458088</v>
@@ -10851,7 +10851,7 @@
         <v>142.5001095249849</v>
       </c>
       <c r="AC97" t="n">
-        <v>106.3351676463896</v>
+        <v>110.2765539912645</v>
       </c>
       <c r="AD97" t="inlineStr">
         <is>
@@ -10937,7 +10937,7 @@
         <v>141.9876776555864</v>
       </c>
       <c r="V98" t="n">
-        <v>183.8699801516967</v>
+        <v>134.1524042530606</v>
       </c>
       <c r="W98" t="n">
         <v>141.9876597644194</v>
@@ -10946,7 +10946,7 @@
         <v>756.1098517946758</v>
       </c>
       <c r="Y98" t="n">
-        <v>979.140625</v>
+        <v>714.3856155160533</v>
       </c>
       <c r="Z98" t="n">
         <v>756.1097565210024</v>
@@ -10958,7 +10958,7 @@
         <v>142.519531754572</v>
       </c>
       <c r="AC98" t="n">
-        <v>184.5587392483313</v>
+        <v>134.654926136668</v>
       </c>
       <c r="AD98" t="inlineStr">
         <is>
@@ -11044,28 +11044,28 @@
         <v>136.0048087767481</v>
       </c>
       <c r="V99" t="n">
-        <v>90.10846709420898</v>
+        <v>110.8401756520711</v>
       </c>
       <c r="W99" t="n">
-        <v>136.1371500065006</v>
+        <v>136.1371500065007</v>
       </c>
       <c r="X99" t="n">
         <v>724.2500018698231</v>
       </c>
       <c r="Y99" t="n">
-        <v>479.84375</v>
+        <v>590.2438167097243</v>
       </c>
       <c r="Z99" t="n">
-        <v>724.954742656254</v>
+        <v>724.9547426562543</v>
       </c>
       <c r="AA99" t="n">
         <v>136.5142695878808</v>
       </c>
       <c r="AB99" t="n">
-        <v>136.6471065550331</v>
+        <v>136.6471065550332</v>
       </c>
       <c r="AC99" t="n">
-        <v>90.44600466474515</v>
+        <v>111.255372190353</v>
       </c>
       <c r="AD99" t="inlineStr">
         <is>
@@ -11151,7 +11151,7 @@
         <v>122.5315882607022</v>
       </c>
       <c r="V100" t="n">
-        <v>142.4687925678709</v>
+        <v>116.9212132125896</v>
       </c>
       <c r="W100" t="n">
         <v>122.5316011052094</v>
@@ -11160,7 +11160,7 @@
         <v>652.50268593516</v>
       </c>
       <c r="Y100" t="n">
-        <v>758.671875</v>
+        <v>622.6264324730058</v>
       </c>
       <c r="Z100" t="n">
         <v>652.5027543344646</v>
@@ -11172,7 +11172,7 @@
         <v>122.9905925883041</v>
       </c>
       <c r="AC100" t="n">
-        <v>143.0024668347998</v>
+        <v>117.359188727262</v>
       </c>
       <c r="AD100" t="inlineStr">
         <is>
@@ -11258,7 +11258,7 @@
         <v>173.9133346912965</v>
       </c>
       <c r="V101" t="n">
-        <v>125.4212447392368</v>
+        <v>143.106761695206</v>
       </c>
       <c r="W101" t="n">
         <v>173.9133367251607</v>
@@ -11267,7 +11267,7 @@
         <v>926.1197020034534</v>
       </c>
       <c r="Y101" t="n">
-        <v>667.890625</v>
+        <v>762.069175035352</v>
       </c>
       <c r="Z101" t="n">
         <v>926.1197128341455</v>
@@ -11279,7 +11279,7 @@
         <v>174.5647992020518</v>
       </c>
       <c r="AC101" t="n">
-        <v>125.891060546875</v>
+        <v>143.6428257325555</v>
       </c>
       <c r="AD101" t="inlineStr">
         <is>
@@ -11365,7 +11365,7 @@
         <v>114.4450921415393</v>
       </c>
       <c r="V102" t="n">
-        <v>126.7138610031662</v>
+        <v>103.6569133119592</v>
       </c>
       <c r="W102" t="n">
         <v>114.6133644928176</v>
@@ -11374,10 +11374,10 @@
         <v>521.2321294192969</v>
       </c>
       <c r="Y102" t="n">
-        <v>577.109375</v>
+        <v>472.0981270896576</v>
       </c>
       <c r="Z102" t="n">
-        <v>521.9985140176922</v>
+        <v>521.9985140176923</v>
       </c>
       <c r="AA102" t="n">
         <v>114.8737923470467</v>
@@ -11386,7 +11386,7 @@
         <v>115.042695030218</v>
       </c>
       <c r="AC102" t="n">
-        <v>127.1885188258495</v>
+        <v>104.0452020468238</v>
       </c>
       <c r="AD102" t="inlineStr">
         <is>
@@ -11472,7 +11472,7 @@
         <v>114.4450921415393</v>
       </c>
       <c r="V103" t="n">
-        <v>126.7138610031662</v>
+        <v>103.6569133119592</v>
       </c>
       <c r="W103" t="n">
         <v>114.6133644928176</v>
@@ -11481,10 +11481,10 @@
         <v>521.2321294192969</v>
       </c>
       <c r="Y103" t="n">
-        <v>577.109375</v>
+        <v>472.0981270896576</v>
       </c>
       <c r="Z103" t="n">
-        <v>521.9985140176922</v>
+        <v>521.9985140176923</v>
       </c>
       <c r="AA103" t="n">
         <v>114.8737923470467</v>
@@ -11493,7 +11493,7 @@
         <v>115.042695030218</v>
       </c>
       <c r="AC103" t="n">
-        <v>127.1885188258495</v>
+        <v>104.0452020468238</v>
       </c>
       <c r="AD103" t="inlineStr">
         <is>
@@ -11579,7 +11579,7 @@
         <v>114.4450921415393</v>
       </c>
       <c r="V104" t="n">
-        <v>126.7138610031662</v>
+        <v>103.6569133119592</v>
       </c>
       <c r="W104" t="n">
         <v>114.6133644928176</v>
@@ -11588,10 +11588,10 @@
         <v>521.2321294192969</v>
       </c>
       <c r="Y104" t="n">
-        <v>577.109375</v>
+        <v>472.0981270896576</v>
       </c>
       <c r="Z104" t="n">
-        <v>521.9985140176922</v>
+        <v>521.9985140176923</v>
       </c>
       <c r="AA104" t="n">
         <v>114.8737923470467</v>
@@ -11600,7 +11600,7 @@
         <v>115.042695030218</v>
       </c>
       <c r="AC104" t="n">
-        <v>127.1885188258495</v>
+        <v>104.0452020468238</v>
       </c>
       <c r="AD104" t="inlineStr">
         <is>
@@ -11686,7 +11686,7 @@
         <v>95.3936019126962</v>
       </c>
       <c r="V105" t="n">
-        <v>102.5100898003142</v>
+        <v>87.85419708945554</v>
       </c>
       <c r="W105" t="n">
         <v>95.39362853858485</v>
@@ -11695,7 +11695,7 @@
         <v>434.4634560339007</v>
       </c>
       <c r="Y105" t="n">
-        <v>466.875</v>
+        <v>400.1257666054041</v>
       </c>
       <c r="Z105" t="n">
         <v>434.4635772996394</v>
@@ -11707,7 +11707,7 @@
         <v>95.75096381083935</v>
       </c>
       <c r="AC105" t="n">
-        <v>102.8940826456311</v>
+        <v>88.18329038338516</v>
       </c>
       <c r="AD105" t="inlineStr">
         <is>
@@ -11793,7 +11793,7 @@
         <v>93.81386402696883</v>
       </c>
       <c r="V106" t="n">
-        <v>113.9000997781269</v>
+        <v>90.36413564431933</v>
       </c>
       <c r="W106" t="n">
         <v>93.81386402696883</v>
@@ -11802,7 +11802,7 @@
         <v>427.2686508509605</v>
       </c>
       <c r="Y106" t="n">
-        <v>518.75</v>
+        <v>411.557105365176</v>
       </c>
       <c r="Z106" t="n">
         <v>427.2686508509605</v>
@@ -11814,7 +11814,7 @@
         <v>94.16528165471703</v>
       </c>
       <c r="AC106" t="n">
-        <v>114.3267584951456</v>
+        <v>90.70263092442542</v>
       </c>
       <c r="AD106" t="inlineStr">
         <is>
@@ -11900,28 +11900,28 @@
         <v>166.5630038123446</v>
       </c>
       <c r="V107" t="n">
-        <v>175.1214034088702</v>
+        <v>155.8168351747937</v>
       </c>
       <c r="W107" t="n">
-        <v>166.6254805025665</v>
+        <v>166.6254805025663</v>
       </c>
       <c r="X107" t="n">
         <v>758.5994954874188</v>
       </c>
       <c r="Y107" t="n">
-        <v>797.578125</v>
+        <v>709.6568256250691</v>
       </c>
       <c r="Z107" t="n">
-        <v>758.8840411824249</v>
+        <v>758.8840411824239</v>
       </c>
       <c r="AA107" t="n">
         <v>167.1869326556713</v>
       </c>
       <c r="AB107" t="n">
-        <v>167.2496433775099</v>
+        <v>167.2496433775096</v>
       </c>
       <c r="AC107" t="n">
-        <v>175.7773911862864</v>
+        <v>156.4005099135787</v>
       </c>
       <c r="AD107" t="inlineStr">
         <is>
@@ -12007,7 +12007,7 @@
         <v>80.41346218240321</v>
       </c>
       <c r="V108" t="n">
-        <v>85.4250748335952</v>
+        <v>66.58783364358995</v>
       </c>
       <c r="W108" t="n">
         <v>80.4134704433576</v>
@@ -12016,7 +12016,7 @@
         <v>366.2374623760637</v>
       </c>
       <c r="Y108" t="n">
-        <v>389.0625</v>
+        <v>303.2696088054325</v>
       </c>
       <c r="Z108" t="n">
         <v>366.2374999999999</v>
@@ -12028,7 +12028,7 @@
         <v>80.71469149757279</v>
       </c>
       <c r="AC108" t="n">
-        <v>85.74506887135924</v>
+        <v>66.83726520446452</v>
       </c>
       <c r="AD108" t="inlineStr">
         <is>
@@ -12114,7 +12114,7 @@
         <v>132.3470316439268</v>
       </c>
       <c r="V109" t="n">
-        <v>122.4426072614865</v>
+        <v>113.9648335894923</v>
       </c>
       <c r="W109" t="n">
         <v>132.3470148144411</v>
@@ -12123,7 +12123,7 @@
         <v>602.7652548068388</v>
       </c>
       <c r="Y109" t="n">
-        <v>557.65625</v>
+        <v>519.0448255946325</v>
       </c>
       <c r="Z109" t="n">
         <v>602.7651781581285</v>
@@ -12135,7 +12135,7 @@
         <v>132.842773884468</v>
       </c>
       <c r="AC109" t="n">
-        <v>122.9012653822816</v>
+        <v>114.3917347930844</v>
       </c>
       <c r="AD109" t="inlineStr">
         <is>
@@ -12221,7 +12221,7 @@
         <v>114.7078513714162</v>
       </c>
       <c r="V110" t="n">
-        <v>83.18641333302182</v>
+        <v>96.67990004295457</v>
       </c>
       <c r="W110" t="n">
         <v>114.7078343639825</v>
@@ -12230,7 +12230,7 @@
         <v>956.7371671764962</v>
       </c>
       <c r="Y110" t="n">
-        <v>693.828125</v>
+        <v>806.3724721902718</v>
       </c>
       <c r="Z110" t="n">
         <v>956.7370253235739</v>
@@ -12242,7 +12242,7 @@
         <v>115.1375187763498</v>
       </c>
       <c r="AC110" t="n">
-        <v>83.49802156212074</v>
+        <v>97.04205356340077</v>
       </c>
       <c r="AD110" t="inlineStr">
         <is>
@@ -12328,7 +12328,7 @@
         <v>133.1094290697119</v>
       </c>
       <c r="V111" t="n">
-        <v>174.1472578186625</v>
+        <v>129.6150774221181</v>
       </c>
       <c r="W111" t="n">
         <v>133.1094211698846</v>
@@ -12337,7 +12337,7 @@
         <v>1110.218146099554</v>
       </c>
       <c r="Y111" t="n">
-        <v>1452.5</v>
+        <v>1081.073008635402</v>
       </c>
       <c r="Z111" t="n">
         <v>1110.21808020992</v>
@@ -12349,7 +12349,7 @@
         <v>133.6080361401092</v>
       </c>
       <c r="AC111" t="n">
-        <v>174.7995965412622</v>
+        <v>130.1006029198738</v>
       </c>
       <c r="AD111" t="inlineStr">
         <is>
@@ -12518,7 +12518,7 @@
         <v>105.6318423342176</v>
       </c>
       <c r="V113" t="n">
-        <v>99.51271875352144</v>
+        <v>95.44570053327124</v>
       </c>
       <c r="W113" t="n">
         <v>105.6318435087638</v>
@@ -12527,7 +12527,7 @@
         <v>881.0374215034507</v>
       </c>
       <c r="Y113" t="n">
-        <v>830</v>
+        <v>796.0784554467998</v>
       </c>
       <c r="Z113" t="n">
         <v>881.0374312999209</v>
@@ -12539,7 +12539,7 @@
         <v>106.0275301404311</v>
       </c>
       <c r="AC113" t="n">
-        <v>99.88548373786409</v>
+        <v>95.80323086216298</v>
       </c>
       <c r="AD113" t="inlineStr">
         <is>
@@ -12708,7 +12708,7 @@
         <v>109.1039483278914</v>
       </c>
       <c r="V115" t="n">
-        <v>81.63152710249805</v>
+        <v>93.64908218816682</v>
       </c>
       <c r="W115" t="n">
         <v>109.1039547787944</v>
@@ -12717,7 +12717,7 @@
         <v>909.997015923609</v>
       </c>
       <c r="Y115" t="n">
-        <v>680.859375</v>
+        <v>781.0935043258265</v>
       </c>
       <c r="Z115" t="n">
         <v>909.9970697282836</v>
@@ -12729,7 +12729,7 @@
         <v>109.512647602227</v>
       </c>
       <c r="AC115" t="n">
-        <v>81.93731087871663</v>
+        <v>93.9998825591429</v>
       </c>
       <c r="AD115" t="inlineStr">
         <is>
@@ -12815,7 +12815,7 @@
         <v>124.9577074028051</v>
       </c>
       <c r="V116" t="n">
-        <v>154.7111799371153</v>
+        <v>117.9593223258183</v>
       </c>
       <c r="W116" t="n">
         <v>124.9577158034129</v>
@@ -12824,7 +12824,7 @@
         <v>1042.227550844179</v>
       </c>
       <c r="Y116" t="n">
-        <v>1290.390625</v>
+        <v>983.8565236362276</v>
       </c>
       <c r="Z116" t="n">
         <v>1042.227620910645</v>
@@ -12836,7 +12836,7 @@
         <v>125.4257952766542</v>
       </c>
       <c r="AC116" t="n">
-        <v>155.2907129987106</v>
+        <v>118.4011864964553</v>
       </c>
       <c r="AD116" t="inlineStr">
         <is>
@@ -13254,7 +13254,7 @@
         <v>119.2005661692046</v>
       </c>
       <c r="V121" t="n">
-        <v>128.886955012091</v>
+        <v>111.3493450454741</v>
       </c>
       <c r="W121" t="n">
         <v>119.2005588392866</v>
@@ -13263,7 +13263,7 @@
         <v>1031.492143197263</v>
       </c>
       <c r="Y121" t="n">
-        <v>1115.3125</v>
+        <v>963.5522569710803</v>
       </c>
       <c r="Z121" t="n">
         <v>1031.49207976843</v>
@@ -13275,7 +13275,7 @@
         <v>119.6470725614111</v>
       </c>
       <c r="AC121" t="n">
-        <v>129.3697530339806</v>
+        <v>111.7664488828766</v>
       </c>
       <c r="AD121" t="inlineStr">
         <is>
@@ -13361,7 +13361,7 @@
         <v>109.1738636564882</v>
       </c>
       <c r="V122" t="n">
-        <v>85.4250748335952</v>
+        <v>93.38022670743987</v>
       </c>
       <c r="W122" t="n">
         <v>109.1738492986071</v>
@@ -13370,7 +13370,7 @@
         <v>944.7269104771252</v>
       </c>
       <c r="Y122" t="n">
-        <v>739.21875</v>
+        <v>808.0579922915497</v>
       </c>
       <c r="Z122" t="n">
         <v>944.7267862324011</v>
@@ -13382,7 +13382,7 @@
         <v>109.5828039401261</v>
       </c>
       <c r="AC122" t="n">
-        <v>85.74506887135924</v>
+        <v>93.73001997188408</v>
       </c>
       <c r="AD122" t="inlineStr">
         <is>
@@ -13800,7 +13800,7 @@
         <v>119.2125459979812</v>
       </c>
       <c r="V127" t="n">
-        <v>148.3323996781594</v>
+        <v>108.1215154419398</v>
       </c>
       <c r="W127" t="n">
         <v>119.2125409772724</v>
@@ -13809,7 +13809,7 @@
         <v>1115.238713129702</v>
       </c>
       <c r="Y127" t="n">
-        <v>1387.65625</v>
+        <v>1011.481624972125</v>
       </c>
       <c r="Z127" t="n">
         <v>1115.238666160746</v>
@@ -13821,7 +13821,7 @@
         <v>119.6590995833226</v>
       </c>
       <c r="AC127" t="n">
-        <v>148.8880384481189</v>
+        <v>108.5265281429861</v>
       </c>
       <c r="AD127" t="inlineStr">
         <is>
@@ -13907,7 +13907,7 @@
         <v>128.3166942407068</v>
       </c>
       <c r="V128" t="n">
-        <v>87.99157379241156</v>
+        <v>107.1706226525133</v>
       </c>
       <c r="W128" t="n">
         <v>128.3167166180678</v>
@@ -13916,7 +13916,7 @@
         <v>1153.639268618678</v>
       </c>
       <c r="Y128" t="n">
-        <v>791.09375</v>
+        <v>963.5241888504934</v>
       </c>
       <c r="Z128" t="n">
         <v>1153.639469803743</v>
@@ -13928,7 +13928,7 @@
         <v>128.7973785822888</v>
       </c>
       <c r="AC128" t="n">
-        <v>88.32118168613472</v>
+        <v>107.5720734014774</v>
       </c>
       <c r="AD128" t="inlineStr">
         <is>
@@ -14014,7 +14014,7 @@
         <v>157.0022533005351</v>
       </c>
       <c r="V129" t="n">
-        <v>126.2174214235412</v>
+        <v>148.6171602139234</v>
       </c>
       <c r="W129" t="n">
         <v>157.0022421272351</v>
@@ -14023,7 +14023,7 @@
         <v>1411.538582262312</v>
       </c>
       <c r="Y129" t="n">
-        <v>1134.765625</v>
+        <v>1336.151878194078</v>
       </c>
       <c r="Z129" t="n">
         <v>1411.538481808059</v>
@@ -14035,7 +14035,7 @@
         <v>157.5903572853917</v>
       </c>
       <c r="AC129" t="n">
-        <v>126.6902196317506</v>
+        <v>149.1738656692071</v>
       </c>
       <c r="AD129" t="inlineStr">
         <is>
@@ -14121,7 +14121,7 @@
         <v>141.4506300739475</v>
       </c>
       <c r="V130" t="n">
-        <v>105.6947965375316</v>
+        <v>124.079768523649</v>
       </c>
       <c r="W130" t="n">
         <v>141.450604047704</v>
@@ -14130,7 +14130,7 @@
         <v>1076.07139584631</v>
       </c>
       <c r="Y130" t="n">
-        <v>804.0625</v>
+        <v>943.924319331269</v>
       </c>
       <c r="Z130" t="n">
         <v>1076.071197854289</v>
@@ -14142,7 +14142,7 @@
         <v>141.980464279276</v>
       </c>
       <c r="AC130" t="n">
-        <v>106.0907189851335</v>
+        <v>124.5445592916061</v>
       </c>
       <c r="AD130" t="inlineStr">
         <is>
@@ -14228,7 +14228,7 @@
         <v>102.0036145991135</v>
       </c>
       <c r="V131" t="n">
-        <v>75.00921044599016</v>
+        <v>92.23047934723739</v>
       </c>
       <c r="W131" t="n">
         <v>102.0036145991135</v>
@@ -14237,7 +14237,7 @@
         <v>775.9822058456383</v>
       </c>
       <c r="Y131" t="n">
-        <v>570.625</v>
+        <v>701.6340655313586</v>
       </c>
       <c r="Z131" t="n">
         <v>775.9822058456383</v>
@@ -14249,7 +14249,7 @@
         <v>102.3857102374923</v>
       </c>
       <c r="AC131" t="n">
-        <v>75.29018766686893</v>
+        <v>92.57596576968098</v>
       </c>
       <c r="AD131" t="inlineStr">
         <is>
@@ -14335,7 +14335,7 @@
         <v>158.1853147488017</v>
       </c>
       <c r="V132" t="n">
-        <v>112.5138156689853</v>
+        <v>144.3172704632135</v>
       </c>
       <c r="W132" t="n">
         <v>158.185312408025</v>
@@ -14344,7 +14344,7 @@
         <v>1203.378820971982</v>
       </c>
       <c r="Y132" t="n">
-        <v>855.9375</v>
+        <v>1097.879073362164</v>
       </c>
       <c r="Z132" t="n">
         <v>1203.37880316476</v>
@@ -14356,7 +14356,7 @@
         <v>158.777859232608</v>
       </c>
       <c r="AC132" t="n">
-        <v>112.9352815003034</v>
+        <v>144.857868948899</v>
       </c>
       <c r="AD132" t="inlineStr">
         <is>
@@ -14442,7 +14442,7 @@
         <v>138.3781947501238</v>
       </c>
       <c r="V133" t="n">
-        <v>106.5471739289633</v>
+        <v>120.7694491830507</v>
       </c>
       <c r="W133" t="n">
         <v>138.3781957891426</v>
@@ -14451,7 +14451,7 @@
         <v>1052.698154130624</v>
       </c>
       <c r="Y133" t="n">
-        <v>810.546875</v>
+        <v>918.7413989605902</v>
       </c>
       <c r="Z133" t="n">
         <v>1052.698162034855</v>
@@ -14463,7 +14463,7 @@
         <v>138.8965470776294</v>
       </c>
       <c r="AC133" t="n">
-        <v>106.9462892995297</v>
+        <v>121.2218398161043</v>
       </c>
       <c r="AD133" t="inlineStr">
         <is>

</xml_diff>